<commit_message>
Completed Semester Validation using RegExp
</commit_message>
<xml_diff>
--- a/Test Cases/Test Cases.xlsx
+++ b/Test Cases/Test Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Projects\CS372-AssignmentOrganizer\Test Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E36073E-D57F-402C-82AE-C38F7716CF98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C64A42-FB51-45B9-BB29-1A00169A9643}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4644" yWindow="3156" windowWidth="23040" windowHeight="11868" xr2:uid="{E8A9AF7F-5AC9-4F24-BE78-E46CAFF50397}"/>
+    <workbookView xWindow="4656" yWindow="3168" windowWidth="23040" windowHeight="11868" xr2:uid="{E8A9AF7F-5AC9-4F24-BE78-E46CAFF50397}"/>
   </bookViews>
   <sheets>
     <sheet name="HomePage" sheetId="1" r:id="rId1"/>
@@ -438,7 +438,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Tested home page on Windows
</commit_message>
<xml_diff>
--- a/Test Cases/Test Cases.xlsx
+++ b/Test Cases/Test Cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SHUBHAM\Downloads\Test Cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University stuff\AssignmentOrganizer\Test Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF020662-EA2D-4FB6-81A6-3D1217C84F07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BAA843C-9C69-4872-BDF0-7201EDA59268}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="2016" windowWidth="23040" windowHeight="14076" xr2:uid="{E8A9AF7F-5AC9-4F24-BE78-E46CAFF50397}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E8A9AF7F-5AC9-4F24-BE78-E46CAFF50397}"/>
   </bookViews>
   <sheets>
     <sheet name="HomePage" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="63">
   <si>
     <t>Test Case#</t>
   </si>
@@ -761,17 +761,17 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="25" style="1" customWidth="1"/>
-    <col min="3" max="4" width="24.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="38.77734375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="41.77734375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" customWidth="1"/>
+    <col min="3" max="4" width="24.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="38.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="41.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -800,7 +800,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -819,13 +819,15 @@
       <c r="F2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="15"/>
+      <c r="G2" s="15" t="s">
+        <v>43</v>
+      </c>
       <c r="H2" s="15"/>
       <c r="I2" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -844,13 +846,15 @@
       <c r="F3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="15"/>
+      <c r="G3" s="15" t="s">
+        <v>43</v>
+      </c>
       <c r="H3" s="17"/>
       <c r="I3" s="16" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -869,13 +873,15 @@
       <c r="F4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="15"/>
+      <c r="G4" s="15" t="s">
+        <v>43</v>
+      </c>
       <c r="H4" s="15"/>
       <c r="I4" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -900,7 +906,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -919,13 +925,15 @@
       <c r="F6" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="G6" s="15"/>
+      <c r="G6" s="15" t="s">
+        <v>43</v>
+      </c>
       <c r="H6" s="17"/>
       <c r="I6" s="16" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -944,13 +952,15 @@
       <c r="F7" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="G7" s="15"/>
+      <c r="G7" s="15" t="s">
+        <v>43</v>
+      </c>
       <c r="H7" s="17"/>
       <c r="I7" s="16" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -969,13 +979,15 @@
       <c r="F8" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G8" s="15"/>
+      <c r="G8" s="15" t="s">
+        <v>43</v>
+      </c>
       <c r="H8" s="17"/>
       <c r="I8" s="16" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -994,13 +1006,15 @@
       <c r="F9" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="G9" s="15"/>
+      <c r="G9" s="15" t="s">
+        <v>43</v>
+      </c>
       <c r="H9" s="17"/>
       <c r="I9" s="16" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -1019,13 +1033,15 @@
       <c r="F10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="15"/>
+      <c r="G10" s="15" t="s">
+        <v>43</v>
+      </c>
       <c r="H10" s="15"/>
       <c r="I10" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -1044,13 +1060,15 @@
       <c r="F11" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="G11" s="15"/>
+      <c r="G11" s="15" t="s">
+        <v>43</v>
+      </c>
       <c r="H11" s="17"/>
       <c r="I11" s="16" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
       <c r="C12" s="6" t="s">
@@ -1065,13 +1083,15 @@
       <c r="F12" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G12" s="15"/>
+      <c r="G12" s="15" t="s">
+        <v>43</v>
+      </c>
       <c r="H12" s="15"/>
       <c r="I12" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="7"/>
       <c r="C13" s="6" t="s">
@@ -1086,13 +1106,15 @@
       <c r="F13" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="G13" s="15"/>
+      <c r="G13" s="15" t="s">
+        <v>43</v>
+      </c>
       <c r="H13" s="17"/>
       <c r="I13" s="16" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="7"/>
       <c r="C14" s="6" t="s">
@@ -1107,13 +1129,15 @@
       <c r="F14" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="15"/>
+      <c r="G14" s="15" t="s">
+        <v>43</v>
+      </c>
       <c r="H14" s="17"/>
       <c r="I14" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="9"/>
       <c r="C15" s="8" t="s">
@@ -1128,7 +1152,9 @@
       <c r="F15" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="G15" s="15"/>
+      <c r="G15" s="15" t="s">
+        <v>43</v>
+      </c>
       <c r="H15" s="15"/>
       <c r="I15" s="2" t="s">
         <v>43</v>
@@ -1146,7 +1172,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1158,7 +1184,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1170,7 +1196,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Test Cases.xlsx (#34)
Added semester test cases.
</commit_message>
<xml_diff>
--- a/Test Cases/Test Cases.xlsx
+++ b/Test Cases/Test Cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University stuff\AssignmentOrganizer\Test Cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\2020 3Fall\CS 372\CS372_Repo\AssignmentOrganizer\Test Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BAA843C-9C69-4872-BDF0-7201EDA59268}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2EDE438-68D0-445F-BCE5-677E4D3CA97B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E8A9AF7F-5AC9-4F24-BE78-E46CAFF50397}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{E8A9AF7F-5AC9-4F24-BE78-E46CAFF50397}"/>
   </bookViews>
   <sheets>
     <sheet name="HomePage" sheetId="1" r:id="rId1"/>
@@ -18,25 +18,17 @@
     <sheet name="CoursesPage" sheetId="3" r:id="rId3"/>
     <sheet name="AssignmentsPage" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="148">
   <si>
     <t>Test Case#</t>
   </si>
@@ -44,6 +36,9 @@
     <t>Test Case Description</t>
   </si>
   <si>
+    <t>Test Steps</t>
+  </si>
+  <si>
     <t>Test Data</t>
   </si>
   <si>
@@ -53,18 +48,48 @@
     <t>Actual Result</t>
   </si>
   <si>
+    <t>Windows OS</t>
+  </si>
+  <si>
+    <t>Linux OS</t>
+  </si>
+  <si>
+    <t>MacOS</t>
+  </si>
+  <si>
+    <t>Default App Window Size</t>
+  </si>
+  <si>
+    <t>Checking the default window size for the app</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>The app window size should be maximized (full screen) when the app launches.</t>
+  </si>
+  <si>
+    <t>The app window size is maximized (full screen) when the app launches.</t>
+  </si>
+  <si>
+    <t>Works</t>
+  </si>
+  <si>
     <t>Check Semester Count</t>
   </si>
   <si>
+    <t>Verify the semester count by going to Semesters Page or semesters.json to find the number of existing semesters.</t>
+  </si>
+  <si>
+    <t>Semester Count on homepage should match the Semester count in Semesters.json and semesters page.</t>
+  </si>
+  <si>
     <t>Semester Count on homepage matches the Semester count in Semesters.json and Semester page.</t>
   </si>
   <si>
     <t>Check Course Count</t>
   </si>
   <si>
-    <t>Verify the semester count by going to Semesters Page or semesters.json to find the number of existing semesters.</t>
-  </si>
-  <si>
     <t>Verify the course count by going to Courses Page or courses.json to find the number of existing courses.</t>
   </si>
   <si>
@@ -74,48 +99,84 @@
     <t>Course Count on homepage matches the course count in courses.json and courses page.</t>
   </si>
   <si>
+    <t>Check Assignment Count</t>
+  </si>
+  <si>
     <t>Verify the assignment count by going to Assignments Page or assignments.json to find the number of existing assignments.</t>
   </si>
   <si>
     <t>Assignment Count on homepage should match the assignment count in assignments.json and assignments page.</t>
   </si>
   <si>
-    <t>Semester Count on homepage should match the Semester count in Semesters.json and semesters page.</t>
-  </si>
-  <si>
     <t>Assignment Count on homepage matches the assignment count in assignments.json and assignments page.</t>
   </si>
   <si>
-    <t>Default App Window Size</t>
-  </si>
-  <si>
-    <t>The app window size should be maximized (full screen) when the app launches.</t>
-  </si>
-  <si>
-    <t>Checking the default window size for the app</t>
-  </si>
-  <si>
-    <t>The app window size is maximized (full screen) when the app launches.</t>
+    <t>Open Semester Page</t>
+  </si>
+  <si>
+    <t>Click on Semesters Card</t>
+  </si>
+  <si>
+    <t>Should redirect to Semester Page</t>
+  </si>
+  <si>
+    <t>It redirects to Semester Page</t>
+  </si>
+  <si>
+    <t>Open Course Page</t>
+  </si>
+  <si>
+    <t>Click on Courses Card</t>
+  </si>
+  <si>
+    <t>Should redirect to Course Page</t>
+  </si>
+  <si>
+    <t>It redirects to Course Page</t>
+  </si>
+  <si>
+    <t>Open Assignment Page</t>
+  </si>
+  <si>
+    <t>Click on Assignments Card</t>
+  </si>
+  <si>
+    <t>Should redirect to Assignment Page</t>
+  </si>
+  <si>
+    <t>It redirects to Assignment Page</t>
+  </si>
+  <si>
+    <t>Open Settings Page</t>
+  </si>
+  <si>
+    <t>Click on Settings Card</t>
+  </si>
+  <si>
+    <t>Should redirect to Settings Page</t>
+  </si>
+  <si>
+    <t>It redirects to Settings Page</t>
+  </si>
+  <si>
+    <t>Checking Exit functionality in the app File Menu</t>
   </si>
   <si>
     <t>Pressing the exit button in the File menu of the app</t>
   </si>
   <si>
+    <t>The app should close/exit when the exit button is pressed.</t>
+  </si>
+  <si>
     <t>The app closes when the exit button is pressed.</t>
   </si>
   <si>
-    <t>The app should close/exit when the exit button is pressed.</t>
-  </si>
-  <si>
-    <t>Checking Exit functionality in the app File Menu</t>
+    <t>Checking the functionality for Go menu in the app</t>
   </si>
   <si>
     <t>Clicking on Home under the Go menu</t>
   </si>
   <si>
-    <t>Checking the functionality for Go menu in the app</t>
-  </si>
-  <si>
     <t>It should redirect to Home page when this button is pressed from anywhere within the app.</t>
   </si>
   <si>
@@ -125,113 +186,308 @@
     <t>Clicking on Semester under the Go menu</t>
   </si>
   <si>
+    <t>It should redirect to Semester page when this button is pressed from anywhere within the app.</t>
+  </si>
+  <si>
+    <t>It redirects to the Semester page when this button is pressed from anywhere within the app.</t>
+  </si>
+  <si>
     <t>Clicking on Course under the Go menu</t>
   </si>
   <si>
+    <t>It should redirect to Course page when this button is pressed from anywhere within the app.</t>
+  </si>
+  <si>
+    <t>It redirects to the Course page when this button is pressed from anywhere within the app.</t>
+  </si>
+  <si>
     <t>Clicking on Assignment under the Go menu</t>
   </si>
   <si>
+    <t>It should redirect to Assignment page when this button is pressed from anywhere within the app.</t>
+  </si>
+  <si>
+    <t>It redirects to the Assignment page when this button is pressed from anywhere within the app.</t>
+  </si>
+  <si>
     <t>Clicking on Settings under the Go menu</t>
   </si>
   <si>
-    <t>It should redirect to Semester page when this button is pressed from anywhere within the app.</t>
-  </si>
-  <si>
-    <t>It redirects to the Semester page when this button is pressed from anywhere within the app.</t>
-  </si>
-  <si>
-    <t>It should redirect to Course page when this button is pressed from anywhere within the app.</t>
-  </si>
-  <si>
-    <t>It redirects to the Course page when this button is pressed from anywhere within the app.</t>
-  </si>
-  <si>
-    <t>It should redirect to Assignment page when this button is pressed from anywhere within the app.</t>
-  </si>
-  <si>
-    <t>It redirects to the Assignment page when this button is pressed from anywhere within the app.</t>
-  </si>
-  <si>
     <t>It should redirect to Settings page when this button is pressed from anywhere within the app.</t>
   </si>
   <si>
     <t>It redirects to the Settings page when this button is pressed from anywhere within the app.</t>
   </si>
   <si>
-    <t>Windows OS</t>
-  </si>
-  <si>
-    <t>Linux OS</t>
-  </si>
-  <si>
-    <t>MacOS</t>
-  </si>
-  <si>
-    <t>Works</t>
-  </si>
-  <si>
-    <t>Check Assignment Count</t>
-  </si>
-  <si>
-    <t>Open Semester Page</t>
-  </si>
-  <si>
-    <t>Open Course Page</t>
-  </si>
-  <si>
-    <t>Open Assignment Page</t>
-  </si>
-  <si>
-    <t>Open Settings Page</t>
-  </si>
-  <si>
-    <t>Click on Settings Card</t>
-  </si>
-  <si>
-    <t>Test Steps</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>Click on Courses Card</t>
-  </si>
-  <si>
-    <t>Click on Semesters Card</t>
-  </si>
-  <si>
-    <t>Click on Assignments Card</t>
-  </si>
-  <si>
-    <t>Should redirect to Semester Page</t>
-  </si>
-  <si>
-    <t>Should redirect to Course Page</t>
-  </si>
-  <si>
-    <t>Should redirect to Assignment Page</t>
-  </si>
-  <si>
-    <t>Should redirect to Settings Page</t>
-  </si>
-  <si>
-    <t>It redirects to Semester Page</t>
-  </si>
-  <si>
-    <t>It redirects to Course Page</t>
-  </si>
-  <si>
-    <t>It redirects to Assignment Page</t>
-  </si>
-  <si>
-    <t>It redirects to Settings Page</t>
+    <t>Adding</t>
+  </si>
+  <si>
+    <t>Adding  semesters with viable years</t>
+  </si>
+  <si>
+    <t>Select a term and enter a viable year</t>
+  </si>
+  <si>
+    <t>1. Fall 2020 
+2. Winter 2020        3. Winter 2019
+4.Spring 2019
+5.Summer 2018</t>
+  </si>
+  <si>
+    <t>It should display a comfirmation dialog box, add semester year if not already existing, entered semesters in the existing semesters year.</t>
+  </si>
+  <si>
+    <t>It displays the the confirmation dialog box, added year if not already an existing year and added semeter to year already existing semester list</t>
+  </si>
+  <si>
+    <t>Adding duplicate semesters</t>
+  </si>
+  <si>
+    <t>Select the terms and enter years of those semesters that you see in existing semesters</t>
+  </si>
+  <si>
+    <t>1. Fall 2020 
+2. Winter 2020
+3.Spring 2019
+4.Summer 2018</t>
+  </si>
+  <si>
+    <t>It should not make any changes and only disply an error message, telling the user that the semester exists.</t>
+  </si>
+  <si>
+    <t>It does not make any changes and displays the error message.</t>
+  </si>
+  <si>
+    <t>Adding semester using non-viable term</t>
+  </si>
+  <si>
+    <t>Leave term unchanged and enter a viable year</t>
+  </si>
+  <si>
+    <t>It should not make any changes and only disply an error message, telling the user that they must select season/term</t>
+  </si>
+  <si>
+    <t>Adding semesters using non-viable years</t>
+  </si>
+  <si>
+    <t>Select a term and enter non-viable year.</t>
+  </si>
+  <si>
+    <t>1.Fall 1996,199
+2.Winter 2022,20
+3.Spring 1999,1
+4.Summer 2025    5. Winter 20AB,        ABCD</t>
+  </si>
+  <si>
+    <t>It should not make any changes and only dispaly an error message, telling the user what years are viable.</t>
+  </si>
+  <si>
+    <t>Adding semester without entering a year</t>
+  </si>
+  <si>
+    <t>Select a term and click add</t>
+  </si>
+  <si>
+    <t>All terms</t>
+  </si>
+  <si>
+    <t>It displays an error message, telling the user what years are viable.</t>
+  </si>
+  <si>
+    <t>The app displays the error message</t>
+  </si>
+  <si>
+    <t>Adding a year more than 4 charcters long</t>
+  </si>
+  <si>
+    <t>Try tying a year more than 4 checters long</t>
+  </si>
+  <si>
+    <t>1. 20201                  2. ABCDE</t>
+  </si>
+  <si>
+    <t>It should not allow you to type more than 4 characters in the year field</t>
+  </si>
+  <si>
+    <t>The app did not allow to type more than 4 charcters</t>
+  </si>
+  <si>
+    <t>Trying to add blank fields</t>
+  </si>
+  <si>
+    <t>Click add</t>
+  </si>
+  <si>
+    <t>It displays an error message, instructing user to select a seanson/term and add a year.</t>
+  </si>
+  <si>
+    <t>The app displays the error message, inform  user to select season/term. Should include year as well.</t>
+  </si>
+  <si>
+    <t>Partially works</t>
+  </si>
+  <si>
+    <t>Editing</t>
+  </si>
+  <si>
+    <t>Edit semester with valid data entery</t>
+  </si>
+  <si>
+    <t>1.Winter 2019 to Winter 2018          2. Spring 2019 to fall 2019                 3. Summer2019 to Winter 2017</t>
+  </si>
+  <si>
+    <t>Edit semester using existing semester term and year</t>
+  </si>
+  <si>
+    <t>Click the edit button update term and/or year matching already existing semester. Or no change at all. click update.</t>
+  </si>
+  <si>
+    <t>1. Winter 2020 to Winter 2020         2. Winter 2020 to Fall 2020               3.Fall 2020 to  Fall 2019                     4. Fall 2020 to Winter 2018</t>
+  </si>
+  <si>
+    <t>The app prompted user for permission, clicked yes app diaplyed error dialog box. No changes were made. No changes were made, user was still able to edit.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edit Semester using invalid  term. </t>
+  </si>
+  <si>
+    <t>Click edit Button and update term with invalid entry. click update.</t>
+  </si>
+  <si>
+    <t>Edit semester with invalid year.</t>
+  </si>
+  <si>
+    <t>Click the edit button update year with invalid entry.</t>
+  </si>
+  <si>
+    <t>All semesters</t>
+  </si>
+  <si>
+    <t>Edit semester using invalid  term and year entries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click the edit button update the term and year with invalid entried.  </t>
+  </si>
+  <si>
+    <t>Edit semester year with only one semeter.</t>
+  </si>
+  <si>
+    <t>Drop down a year containing one semester and edit it's year and click update.</t>
+  </si>
+  <si>
+    <t>1. Fall 2019 to Fall 2018</t>
+  </si>
+  <si>
+    <t>It should display a confirmation dialog box for user permission (yes/no) before making changes. Clicking yes it should display a confirmation dialog box letting user know semester was successfuly updated. Semester should be saved under the updated year. And the year edited should be removed from the list of exsiting semester year.</t>
+  </si>
+  <si>
+    <t>Clicking no after clicking on update.</t>
+  </si>
+  <si>
+    <t>Click the edit button to edit a semeter then click on update, then no.</t>
+  </si>
+  <si>
+    <t>1. Winter 2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It should take user back to the edit page and make no changes. </t>
+  </si>
+  <si>
+    <t>Took user back to the update page and made no changes.</t>
+  </si>
+  <si>
+    <t>Clicking cancel under the edit field with or with or witout changes</t>
+  </si>
+  <si>
+    <t>Click the dit button, try editing and not edit the semester field and click on cancel.</t>
+  </si>
+  <si>
+    <t>1. Winter 2017        2.Winter 2017 to Winter 2016</t>
+  </si>
+  <si>
+    <t>It should take user back to the add semeter field and make no changes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Took user back to the add semester field and made no changes. </t>
+  </si>
+  <si>
+    <t>Deleting</t>
+  </si>
+  <si>
+    <t>Delete semesters in exisitng semesters year with multiple semesters</t>
+  </si>
+  <si>
+    <t>1. Winter 2020      2.Fall 2018</t>
+  </si>
+  <si>
+    <t>It asks for confirmation and the semester is deleted. A message is shown confirming deletion. Semster was removed from below the existing semester year</t>
+  </si>
+  <si>
+    <t>It does as expected. The confirmation message is flashed momentarily before fading.</t>
+  </si>
+  <si>
+    <t>Deleting semster in existing semesters year with only one semster.</t>
+  </si>
+  <si>
+    <t>Winter 2017</t>
+  </si>
+  <si>
+    <t>It asks for confirmation and the semester is deleted. A message is shown confirming deletion. Year should be removed from existing semester.</t>
+  </si>
+  <si>
+    <t>It does as expected. The confirmation message is flashed momentarily before fading. Year was also removed from existing semester list.</t>
+  </si>
+  <si>
+    <t>Click the edit button and modify semester term and/or year. click update.</t>
+  </si>
+  <si>
+    <t>Click the delete icon</t>
+  </si>
+  <si>
+    <t>It should display a confirmation dialog box for user permission (yes/no) before making changes. Clicking yes it should display a an error dialog box letting user knwo semester already exist. No changes should be made. User should still be able to edit.</t>
+  </si>
+  <si>
+    <t>It should display a confirmation dialog box for user permission (yes/no) before making changes. Clicking yes it should display error dialog box telling user to select season/term. No changes should be made. User should still be able to edit.</t>
+  </si>
+  <si>
+    <t>It should display a confirmation dialog box for user permission (yes/no) before making changes. Clicking yes it should display error dialog box telling user what year are valid entry. No changes should be made. User should still be able to edit.</t>
+  </si>
+  <si>
+    <t>It should display a confirmation dialog box for user permission (yes/no) before making changes. Clicking yes, it should display error dialog box telling user what term and year are valid entries. No changes should be made. User should still be able to edit.</t>
+  </si>
+  <si>
+    <t>Select Term and enter 2020</t>
+  </si>
+  <si>
+    <t>It should display a confirmation dialog box for user permission (yes/no) before making changes. Clicking yes, it should display a confirmation dialog box letting user know semester was successfuly updated. Semester should be updated with current information and displayed under the correct year or semester.</t>
+  </si>
+  <si>
+    <t>It prompted user for permission. Clicking yes, the app confirmed that the semester was successfully updated. Added semester with updated information under the correct field.</t>
+  </si>
+  <si>
+    <t>It prompted user for permission. Clicking yes, the app displayed error dialog box.  No changes were made, user was still able to edit.</t>
+  </si>
+  <si>
+    <t>It prompted user for permission. Clicking yes, the app displayed error dialog box. No changes were made, user was still able to edit.</t>
+  </si>
+  <si>
+    <t>It prompted user for permission. Clicking yes, the app displayed error dialog box. Was only asking for term and not year. No changes were made, user was still able to edit.</t>
+  </si>
+  <si>
+    <t>Promted user for permission, confirmed semester was successfully updated. Added semester under the new year and removed edited year.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Re-adding deleted semesters </t>
+  </si>
+  <si>
+    <t>It displays the confirmation dialog box and adds the semester to existing semesters. This confirms proprer deletion of the semester.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,8 +503,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -261,8 +525,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -384,11 +666,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -440,6 +757,48 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -757,8 +1116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB585F97-6C77-4717-A37E-33269E5DB975}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,25 +1138,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -805,26 +1164,26 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="H2" s="15"/>
       <c r="I2" s="2" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -832,26 +1191,26 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="H3" s="17"/>
       <c r="I3" s="16" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -859,26 +1218,26 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="H4" s="15"/>
       <c r="I4" s="2" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -886,24 +1245,24 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="G5" s="15"/>
       <c r="H5" s="17"/>
       <c r="I5" s="16" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -911,26 +1270,26 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="H6" s="17"/>
       <c r="I6" s="16" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -938,26 +1297,26 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="H7" s="17"/>
       <c r="I7" s="16" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -965,26 +1324,26 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="H8" s="17"/>
       <c r="I8" s="16" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -992,26 +1351,26 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="H9" s="17"/>
       <c r="I9" s="16" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1019,26 +1378,26 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="H10" s="15"/>
       <c r="I10" s="2" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -1046,118 +1405,118 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="H11" s="17"/>
       <c r="I11" s="16" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
       <c r="C12" s="6" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="H12" s="15"/>
       <c r="I12" s="2" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="7"/>
       <c r="C13" s="6" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="H13" s="17"/>
       <c r="I13" s="16" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="7"/>
       <c r="C14" s="6" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="H14" s="17"/>
       <c r="I14" s="2" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="9"/>
       <c r="C15" s="8" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="H15" s="15"/>
       <c r="I15" s="2" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1168,12 +1527,737 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9381720-3E95-49AA-9890-671A6D04A327}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="28"/>
+    </row>
+    <row r="3" spans="1:12" s="18" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3" s="20">
+        <v>1</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="L3"/>
+    </row>
+    <row r="4" spans="1:12" s="18" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="20">
+        <v>2</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+    </row>
+    <row r="5" spans="1:12" s="18" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="20">
+        <v>3</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+    </row>
+    <row r="6" spans="1:12" s="18" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A6" s="20">
+        <v>4</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+    </row>
+    <row r="7" spans="1:12" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="20">
+        <v>5</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+    </row>
+    <row r="8" spans="1:12" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="20">
+        <v>6</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+    </row>
+    <row r="9" spans="1:12" s="18" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="21">
+        <v>7</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+    </row>
+    <row r="10" spans="1:12" s="18" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A10" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="25"/>
+    </row>
+    <row r="11" spans="1:12" s="18" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="A11" s="20">
+        <v>8</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="G11" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+    </row>
+    <row r="12" spans="1:12" s="18" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A12" s="20">
+        <v>9</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+    </row>
+    <row r="13" spans="1:12" s="18" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A13" s="20">
+        <v>10</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="G13" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+    </row>
+    <row r="14" spans="1:12" s="18" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A14" s="20">
+        <v>11</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="G14" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+    </row>
+    <row r="15" spans="1:12" s="18" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A15" s="21">
+        <v>12</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="G15" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+    </row>
+    <row r="16" spans="1:12" s="18" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A16" s="20">
+        <v>13</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="F16" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="G16" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+    </row>
+    <row r="17" spans="1:9" s="18" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="20">
+        <v>14</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="G17" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+    </row>
+    <row r="18" spans="1:9" s="18" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A18" s="20">
+        <v>15</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="G18" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+    </row>
+    <row r="19" spans="1:9" s="18" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A19" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="25"/>
+    </row>
+    <row r="20" spans="1:9" s="18" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" s="20">
+        <v>16</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="F20" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="G20" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+    </row>
+    <row r="21" spans="1:9" s="18" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A21" s="20">
+        <v>17</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G21" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+    </row>
+    <row r="22" spans="1:9" s="18" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A22" s="20">
+        <v>18</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="F22" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="G22" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+    </row>
+    <row r="23" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="29"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+    </row>
+    <row r="24" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="29"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="22"/>
+    </row>
+    <row r="25" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="29"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="22"/>
+    </row>
+    <row r="26" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="29"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="22"/>
+    </row>
+    <row r="27" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="29"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
+    </row>
+    <row r="28" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="29"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
+    </row>
+    <row r="29" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="29"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="22"/>
+    </row>
+    <row r="30" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="7"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="22"/>
+    </row>
+    <row r="31" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="7"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="22"/>
+    </row>
+    <row r="32" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="7"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="22"/>
+    </row>
+    <row r="33" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="7"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="22"/>
+    </row>
+    <row r="34" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="7"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="22"/>
+    </row>
+    <row r="35" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="7"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="22"/>
+    </row>
+    <row r="36" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="7"/>
+      <c r="B36" s="22"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="22"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="30"/>
+      <c r="B37" s="31"/>
+      <c r="C37" s="31"/>
+      <c r="D37" s="31"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
+      <c r="G37" s="31"/>
+      <c r="H37" s="31"/>
+      <c r="I37" s="31"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="30"/>
+      <c r="B38" s="31"/>
+      <c r="C38" s="31"/>
+      <c r="D38" s="31"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="31"/>
+      <c r="G38" s="31"/>
+      <c r="H38" s="31"/>
+      <c r="I38" s="31"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="30"/>
+      <c r="B39" s="31"/>
+      <c r="C39" s="31"/>
+      <c r="D39" s="31"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="31"/>
+      <c r="G39" s="31"/>
+      <c r="H39" s="31"/>
+      <c r="I39" s="31"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A19:I19"/>
+    <mergeCell ref="A2:I2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1200,4 +2284,207 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C39443884A93AC4288025566ACBEDC04" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="09db1439c13fea15c4b073f8145b668d">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="dcc1e875-6396-4c7a-abb6-a5f631e4ec10" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e59e1d6e6415753d6d52256061396b9c" ns3:_="">
+    <xsd:import namespace="dcc1e875-6396-4c7a-abb6-a5f631e4ec10"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="dcc1e875-6396-4c7a-abb6-a5f631e4ec10" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="11" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1466FD4-D063-4F72-96C2-762D063A7051}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="dcc1e875-6396-4c7a-abb6-a5f631e4ec10"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C0AF795-75F8-4DF0-B47D-DF453830802B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="dcc1e875-6396-4c7a-abb6-a5f631e4ec10"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DAB9CD3-C2C1-49ED-B183-8472C4A927BC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added test case 8 to 11 for course page
</commit_message>
<xml_diff>
--- a/Test Cases/Test Cases.xlsx
+++ b/Test Cases/Test Cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23505"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uregina-my.sharepoint.com/personal/sfz421_uregina_ca/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University stuff\AssignmentOrganizer\Test Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{895B2A64-2E8B-4EBB-8ACB-FAE527D8706A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1639DA9-9DB3-4D41-B554-43E4432EB8D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HomePage" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="CoursesPage" sheetId="3" r:id="rId3"/>
     <sheet name="AssignmentsPage" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191028" iterateDelta="1E-4" calcCompleted="0"/>
+  <calcPr calcId="191028" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="253">
   <si>
     <t>Test Case#</t>
   </si>
@@ -577,9 +577,6 @@
   </si>
   <si>
     <t>Results should show up as soon as letter is typed in.</t>
-  </si>
-  <si>
-    <t>Select semster from the drop down.</t>
   </si>
   <si>
     <t>Enter a semester in the database.</t>
@@ -769,12 +766,74 @@
   <si>
     <t xml:space="preserve">It gets deleted. A pop up confirms the deletion to the user and it's deleted in the Json file. </t>
   </si>
+  <si>
+    <t>Select semester from the drop down.</t>
+  </si>
+  <si>
+    <t>Adding an existing course code with different character cases.</t>
+  </si>
+  <si>
+    <t>1.Choose a semester.
+2.Enter a course code different letter cases
+3.Existing course name same letter cases</t>
+  </si>
+  <si>
+    <t>A dialogue shouls appear telling user course code already exist.</t>
+  </si>
+  <si>
+    <t>Adds the course to the semester</t>
+  </si>
+  <si>
+    <t>Dose not work</t>
+  </si>
+  <si>
+    <t>Adding an existing course to a semester with matching cases</t>
+  </si>
+  <si>
+    <t>Semester: Fall 2019, Course Code: cs-200, Course Name: Intro to DBMS.</t>
+  </si>
+  <si>
+    <t>Semester: Fall 2019, Course Code: CS-200, Course Name: Intro to DBMS.</t>
+  </si>
+  <si>
+    <t>A dialogue shouls appear telling user course already exist.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A warning dialogue box appeared. </t>
+  </si>
+  <si>
+    <t>Adding an existing course name with different character cases.</t>
+  </si>
+  <si>
+    <t>1.Choose a semester.
+2.Existing course code
+3.Existing course name differnt letter cases</t>
+  </si>
+  <si>
+    <t>Semester: Fall 2019, Course Code: CS-200, Course Name: intro to dbms.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adding a valid course spelling existing semester name in lower case or a different case sequence </t>
+  </si>
+  <si>
+    <t>1. Type semester term and year                   2.Enter a course code
+3.Enter a course name</t>
+  </si>
+  <si>
+    <t>1. fall 2019:MATH-100: Intro to Calculus                                                    2.fALL 2019:ENGL-100:Critical Read and Writing1</t>
+  </si>
+  <si>
+    <t>Result to appear in existing course list</t>
+  </si>
+  <si>
+    <t>A warning dialogue popped up saying semesters dose not exist</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1000,7 +1059,7 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1093,6 +1152,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1500,7 +1562,7 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="25" style="1" customWidth="1"/>
@@ -1510,7 +1572,7 @@
     <col min="7" max="7" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30">
+    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1539,7 +1601,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="49.9" customHeight="1">
+    <row r="2" spans="1:9" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -1568,7 +1630,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="75">
+    <row r="3" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="30">
         <v>2</v>
       </c>
@@ -1597,7 +1659,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="75">
+    <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="30">
         <v>3</v>
       </c>
@@ -1626,7 +1688,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="90">
+    <row r="5" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="30">
         <v>4</v>
       </c>
@@ -1651,7 +1713,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="30">
         <v>5</v>
       </c>
@@ -1680,7 +1742,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="30">
         <v>6</v>
       </c>
@@ -1709,7 +1771,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="30">
         <v>7</v>
       </c>
@@ -1738,7 +1800,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="30">
         <v>8</v>
       </c>
@@ -1767,7 +1829,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="45">
+    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="30">
         <v>9</v>
       </c>
@@ -1796,7 +1858,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="28.9" customHeight="1">
+    <row r="11" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>10</v>
       </c>
@@ -1825,7 +1887,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="28.9" customHeight="1">
+    <row r="12" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="9"/>
       <c r="C12" s="13" t="s">
@@ -1850,7 +1912,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="28.9" customHeight="1">
+    <row r="13" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
       <c r="B13" s="9"/>
       <c r="C13" s="13" t="s">
@@ -1875,7 +1937,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="28.9" customHeight="1">
+    <row r="14" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
       <c r="B14" s="9"/>
       <c r="C14" s="13" t="s">
@@ -1900,7 +1962,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="28.9" customHeight="1">
+    <row r="15" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
       <c r="B15" s="16"/>
       <c r="C15" s="15" t="s">
@@ -1939,7 +2001,7 @@
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
@@ -1951,7 +2013,7 @@
     <col min="9" max="9" width="7.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39" customHeight="1">
+    <row r="1" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1980,20 +2042,20 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="22.5" customHeight="1">
-      <c r="A2" s="32" t="s">
+    <row r="2" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-    </row>
-    <row r="3" spans="1:9" s="21" customFormat="1" ht="90">
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+    </row>
+    <row r="3" spans="1:9" s="21" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="18">
         <v>1</v>
       </c>
@@ -2020,7 +2082,7 @@
       </c>
       <c r="I3" s="19"/>
     </row>
-    <row r="4" spans="1:9" s="21" customFormat="1" ht="75">
+    <row r="4" spans="1:9" s="21" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="18">
         <v>2</v>
       </c>
@@ -2047,7 +2109,7 @@
       </c>
       <c r="I4" s="19"/>
     </row>
-    <row r="5" spans="1:9" s="21" customFormat="1" ht="60">
+    <row r="5" spans="1:9" s="21" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="18">
         <v>3</v>
       </c>
@@ -2074,7 +2136,7 @@
       </c>
       <c r="I5" s="19"/>
     </row>
-    <row r="6" spans="1:9" s="21" customFormat="1" ht="105">
+    <row r="6" spans="1:9" s="21" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="18">
         <v>4</v>
       </c>
@@ -2101,7 +2163,7 @@
       </c>
       <c r="I6" s="19"/>
     </row>
-    <row r="7" spans="1:9" s="21" customFormat="1" ht="45">
+    <row r="7" spans="1:9" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="18">
         <v>5</v>
       </c>
@@ -2128,7 +2190,7 @@
       </c>
       <c r="I7" s="19"/>
     </row>
-    <row r="8" spans="1:9" s="21" customFormat="1" ht="45">
+    <row r="8" spans="1:9" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="18">
         <v>6</v>
       </c>
@@ -2155,7 +2217,7 @@
       </c>
       <c r="I8" s="19"/>
     </row>
-    <row r="9" spans="1:9" s="21" customFormat="1" ht="75">
+    <row r="9" spans="1:9" s="21" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="28">
         <v>7</v>
       </c>
@@ -2182,7 +2244,7 @@
       </c>
       <c r="I9" s="19"/>
     </row>
-    <row r="10" spans="1:9" s="21" customFormat="1" ht="60">
+    <row r="10" spans="1:9" s="21" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="31">
         <v>8</v>
       </c>
@@ -2207,7 +2269,7 @@
       <c r="H10" s="19"/>
       <c r="I10" s="19"/>
     </row>
-    <row r="11" spans="1:9" s="21" customFormat="1" ht="45">
+    <row r="11" spans="1:9" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="28">
         <v>9</v>
       </c>
@@ -2232,20 +2294,20 @@
       <c r="H11" s="19"/>
       <c r="I11" s="19"/>
     </row>
-    <row r="12" spans="1:9" s="21" customFormat="1" ht="21" customHeight="1">
-      <c r="A12" s="33" t="s">
+    <row r="12" spans="1:9" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="B12" s="33"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-    </row>
-    <row r="13" spans="1:9" s="21" customFormat="1" ht="150">
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+    </row>
+    <row r="13" spans="1:9" s="21" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A13" s="18">
         <v>10</v>
       </c>
@@ -2272,7 +2334,7 @@
       </c>
       <c r="I13" s="19"/>
     </row>
-    <row r="14" spans="1:9" s="21" customFormat="1" ht="135">
+    <row r="14" spans="1:9" s="21" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A14" s="18">
         <v>11</v>
       </c>
@@ -2299,7 +2361,7 @@
       </c>
       <c r="I14" s="19"/>
     </row>
-    <row r="15" spans="1:9" s="21" customFormat="1" ht="120">
+    <row r="15" spans="1:9" s="21" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A15" s="18">
         <v>12</v>
       </c>
@@ -2326,7 +2388,7 @@
       </c>
       <c r="I15" s="19"/>
     </row>
-    <row r="16" spans="1:9" s="21" customFormat="1" ht="120">
+    <row r="16" spans="1:9" s="21" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A16" s="18">
         <v>13</v>
       </c>
@@ -2353,7 +2415,7 @@
       </c>
       <c r="I16" s="19"/>
     </row>
-    <row r="17" spans="1:9" s="21" customFormat="1" ht="120">
+    <row r="17" spans="1:9" s="21" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A17" s="28">
         <v>14</v>
       </c>
@@ -2380,7 +2442,7 @@
       </c>
       <c r="I17" s="19"/>
     </row>
-    <row r="18" spans="1:9" s="21" customFormat="1" ht="165">
+    <row r="18" spans="1:9" s="21" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A18" s="18">
         <v>15</v>
       </c>
@@ -2407,7 +2469,7 @@
       </c>
       <c r="I18" s="19"/>
     </row>
-    <row r="19" spans="1:9" s="21" customFormat="1" ht="60">
+    <row r="19" spans="1:9" s="21" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="18">
         <v>16</v>
       </c>
@@ -2434,7 +2496,7 @@
       </c>
       <c r="I19" s="19"/>
     </row>
-    <row r="20" spans="1:9" s="21" customFormat="1" ht="75">
+    <row r="20" spans="1:9" s="21" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="18">
         <v>17</v>
       </c>
@@ -2461,22 +2523,22 @@
       </c>
       <c r="I20" s="19"/>
     </row>
-    <row r="21" spans="1:9" s="21" customFormat="1" ht="19.7" customHeight="1">
-      <c r="A21" s="33" t="s">
+    <row r="21" spans="1:9" s="21" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="B21" s="33"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="I21" s="33"/>
-    </row>
-    <row r="22" spans="1:9" s="21" customFormat="1" ht="75">
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" s="34"/>
+    </row>
+    <row r="22" spans="1:9" s="21" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="18">
         <v>18</v>
       </c>
@@ -2503,7 +2565,7 @@
       </c>
       <c r="I22" s="19"/>
     </row>
-    <row r="23" spans="1:9" s="21" customFormat="1" ht="30">
+    <row r="23" spans="1:9" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="18">
         <v>19</v>
       </c>
@@ -2528,7 +2590,7 @@
       </c>
       <c r="I23" s="19"/>
     </row>
-    <row r="24" spans="1:9" s="21" customFormat="1" ht="90">
+    <row r="24" spans="1:9" s="21" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A24" s="18">
         <v>20</v>
       </c>
@@ -2555,7 +2617,7 @@
       </c>
       <c r="I24" s="19"/>
     </row>
-    <row r="25" spans="1:9" s="21" customFormat="1" ht="90">
+    <row r="25" spans="1:9" s="21" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" s="18">
         <v>21</v>
       </c>
@@ -2582,7 +2644,7 @@
       </c>
       <c r="I25" s="19"/>
     </row>
-    <row r="26" spans="1:9" s="21" customFormat="1">
+    <row r="26" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="23"/>
       <c r="B26" s="22"/>
       <c r="C26" s="22"/>
@@ -2593,7 +2655,7 @@
       <c r="H26" s="22"/>
       <c r="I26" s="22"/>
     </row>
-    <row r="27" spans="1:9" s="21" customFormat="1">
+    <row r="27" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="23"/>
       <c r="B27" s="22"/>
       <c r="C27" s="22"/>
@@ -2604,7 +2666,7 @@
       <c r="H27" s="22"/>
       <c r="I27" s="22"/>
     </row>
-    <row r="28" spans="1:9" s="21" customFormat="1">
+    <row r="28" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="23"/>
       <c r="B28" s="22"/>
       <c r="C28" s="22"/>
@@ -2615,7 +2677,7 @@
       <c r="H28" s="22"/>
       <c r="I28" s="22"/>
     </row>
-    <row r="29" spans="1:9" s="21" customFormat="1">
+    <row r="29" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="23"/>
       <c r="B29" s="22"/>
       <c r="C29" s="22"/>
@@ -2626,7 +2688,7 @@
       <c r="H29" s="22"/>
       <c r="I29" s="22"/>
     </row>
-    <row r="30" spans="1:9" s="21" customFormat="1">
+    <row r="30" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="23"/>
       <c r="B30" s="22"/>
       <c r="C30" s="22"/>
@@ -2637,7 +2699,7 @@
       <c r="H30" s="22"/>
       <c r="I30" s="22"/>
     </row>
-    <row r="31" spans="1:9" s="21" customFormat="1">
+    <row r="31" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="23"/>
       <c r="B31" s="22"/>
       <c r="C31" s="22"/>
@@ -2648,7 +2710,7 @@
       <c r="H31" s="22"/>
       <c r="I31" s="22"/>
     </row>
-    <row r="32" spans="1:9" s="21" customFormat="1">
+    <row r="32" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="23"/>
       <c r="B32" s="22"/>
       <c r="C32" s="22"/>
@@ -2659,7 +2721,7 @@
       <c r="H32" s="22"/>
       <c r="I32" s="22"/>
     </row>
-    <row r="33" spans="1:9" s="21" customFormat="1">
+    <row r="33" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
       <c r="B33" s="22"/>
       <c r="C33" s="22"/>
@@ -2670,7 +2732,7 @@
       <c r="H33" s="22"/>
       <c r="I33" s="22"/>
     </row>
-    <row r="34" spans="1:9" s="21" customFormat="1">
+    <row r="34" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="9"/>
       <c r="B34" s="22"/>
       <c r="C34" s="22"/>
@@ -2681,7 +2743,7 @@
       <c r="H34" s="22"/>
       <c r="I34" s="22"/>
     </row>
-    <row r="35" spans="1:9" s="21" customFormat="1">
+    <row r="35" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="9"/>
       <c r="B35" s="22"/>
       <c r="C35" s="22"/>
@@ -2692,7 +2754,7 @@
       <c r="H35" s="22"/>
       <c r="I35" s="22"/>
     </row>
-    <row r="36" spans="1:9" s="21" customFormat="1">
+    <row r="36" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="9"/>
       <c r="B36" s="22"/>
       <c r="C36" s="22"/>
@@ -2703,7 +2765,7 @@
       <c r="H36" s="22"/>
       <c r="I36" s="22"/>
     </row>
-    <row r="37" spans="1:9" s="21" customFormat="1">
+    <row r="37" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="9"/>
       <c r="B37" s="22"/>
       <c r="C37" s="22"/>
@@ -2714,7 +2776,7 @@
       <c r="H37" s="22"/>
       <c r="I37" s="22"/>
     </row>
-    <row r="38" spans="1:9" s="21" customFormat="1">
+    <row r="38" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="9"/>
       <c r="B38" s="22"/>
       <c r="C38" s="22"/>
@@ -2725,7 +2787,7 @@
       <c r="H38" s="22"/>
       <c r="I38" s="22"/>
     </row>
-    <row r="39" spans="1:9" s="21" customFormat="1">
+    <row r="39" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="9"/>
       <c r="B39" s="22"/>
       <c r="C39" s="22"/>
@@ -2736,7 +2798,7 @@
       <c r="H39" s="22"/>
       <c r="I39" s="22"/>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="24"/>
       <c r="B40" s="25"/>
       <c r="C40" s="25"/>
@@ -2747,7 +2809,7 @@
       <c r="H40" s="25"/>
       <c r="I40" s="25"/>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="24"/>
       <c r="B41" s="25"/>
       <c r="C41" s="25"/>
@@ -2758,7 +2820,7 @@
       <c r="H41" s="25"/>
       <c r="I41" s="25"/>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="24"/>
       <c r="B42" s="25"/>
       <c r="C42" s="25"/>
@@ -2782,13 +2844,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:P25"/>
+  <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.42578125" customWidth="1"/>
@@ -2802,7 +2864,7 @@
     <col min="10" max="10" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2834,7 +2896,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="90">
+    <row r="2" spans="1:16" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="26">
         <v>1</v>
       </c>
@@ -2865,7 +2927,7 @@
       <c r="O2" s="21"/>
       <c r="P2" s="21"/>
     </row>
-    <row r="3" spans="1:16" ht="45">
+    <row r="3" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="26">
         <v>2</v>
       </c>
@@ -2891,7 +2953,7 @@
       <c r="I3" s="27"/>
       <c r="J3" s="30"/>
     </row>
-    <row r="4" spans="1:16" ht="45">
+    <row r="4" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="26">
         <v>3</v>
       </c>
@@ -2917,19 +2979,19 @@
       <c r="I4" s="27"/>
       <c r="J4" s="30"/>
     </row>
-    <row r="5" spans="1:16" ht="60">
+    <row r="5" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="26"/>
       <c r="B5" s="27" t="s">
+        <v>234</v>
+      </c>
+      <c r="C5" s="27" t="s">
         <v>177</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="D5" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="E5" s="27" t="s">
         <v>179</v>
-      </c>
-      <c r="E5" s="27" t="s">
-        <v>180</v>
       </c>
       <c r="F5" s="27" t="s">
         <v>101</v>
@@ -2941,21 +3003,21 @@
       <c r="I5" s="27"/>
       <c r="J5" s="30"/>
     </row>
-    <row r="6" spans="1:16" ht="45">
+    <row r="6" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="26">
         <v>4</v>
       </c>
       <c r="B6" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="C6" s="27" t="s">
         <v>181</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="D6" s="27" t="s">
         <v>182</v>
       </c>
-      <c r="D6" s="27" t="s">
+      <c r="E6" s="27" t="s">
         <v>183</v>
-      </c>
-      <c r="E6" s="27" t="s">
-        <v>184</v>
       </c>
       <c r="F6" s="27" t="s">
         <v>101</v>
@@ -2967,24 +3029,24 @@
       <c r="I6" s="27"/>
       <c r="J6" s="30"/>
     </row>
-    <row r="7" spans="1:16" ht="75">
+    <row r="7" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="28">
         <v>5</v>
       </c>
       <c r="B7" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>181</v>
+      </c>
+      <c r="D7" s="27" t="s">
         <v>185</v>
       </c>
-      <c r="C7" s="27" t="s">
-        <v>182</v>
-      </c>
-      <c r="D7" s="27" t="s">
+      <c r="E7" s="27" t="s">
         <v>186</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="F7" s="27" t="s">
         <v>187</v>
-      </c>
-      <c r="F7" s="27" t="s">
-        <v>188</v>
       </c>
       <c r="G7" s="27" t="s">
         <v>96</v>
@@ -2992,27 +3054,27 @@
       <c r="H7" s="27"/>
       <c r="I7" s="27"/>
       <c r="J7" s="30" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="75">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="26">
         <v>6</v>
       </c>
       <c r="B8" s="27" t="s">
+        <v>189</v>
+      </c>
+      <c r="C8" s="27" t="s">
         <v>190</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="D8" s="27" t="s">
         <v>191</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="E8" s="27" t="s">
         <v>192</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="F8" s="27" t="s">
         <v>193</v>
-      </c>
-      <c r="F8" s="27" t="s">
-        <v>194</v>
       </c>
       <c r="G8" s="27" t="s">
         <v>14</v>
@@ -3021,24 +3083,24 @@
       <c r="I8" s="27"/>
       <c r="J8" s="30"/>
     </row>
-    <row r="9" spans="1:16" ht="90">
+    <row r="9" spans="1:16" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="28">
         <v>7</v>
       </c>
       <c r="B9" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="C9" s="27" t="s">
         <v>195</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="D9" s="27" t="s">
         <v>196</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="E9" s="27" t="s">
         <v>197</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="F9" s="27" t="s">
         <v>198</v>
-      </c>
-      <c r="F9" s="27" t="s">
-        <v>199</v>
       </c>
       <c r="G9" s="27" t="s">
         <v>96</v>
@@ -3046,117 +3108,129 @@
       <c r="H9" s="27"/>
       <c r="I9" s="27"/>
       <c r="J9" s="30" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="60">
-      <c r="A10" s="26">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="28">
         <v>8</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>201</v>
+        <v>248</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>202</v>
-      </c>
-      <c r="D10" s="27"/>
+        <v>249</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>250</v>
+      </c>
       <c r="E10" s="27" t="s">
-        <v>203</v>
+        <v>251</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>204</v>
+        <v>252</v>
       </c>
       <c r="G10" s="27" t="s">
-        <v>14</v>
+        <v>239</v>
       </c>
       <c r="H10" s="27"/>
       <c r="I10" s="27"/>
-      <c r="J10" s="30"/>
-    </row>
-    <row r="11" spans="1:16">
-      <c r="A11" s="34" t="s">
-        <v>107</v>
-      </c>
-      <c r="B11" s="34"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="30"/>
-    </row>
-    <row r="12" spans="1:16" ht="120">
-      <c r="A12" s="26">
+      <c r="J10" s="32"/>
+    </row>
+    <row r="11" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="28">
         <v>9</v>
       </c>
+      <c r="B11" s="27" t="s">
+        <v>240</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>181</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>242</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>243</v>
+      </c>
+      <c r="F11" s="27" t="s">
+        <v>244</v>
+      </c>
+      <c r="G11" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="32"/>
+    </row>
+    <row r="12" spans="1:16" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="28">
+        <v>10</v>
+      </c>
       <c r="B12" s="27" t="s">
-        <v>205</v>
+        <v>235</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>206</v>
+        <v>236</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>207</v>
+        <v>241</v>
       </c>
       <c r="E12" s="27" t="s">
-        <v>208</v>
+        <v>237</v>
       </c>
       <c r="F12" s="27" t="s">
-        <v>101</v>
+        <v>238</v>
       </c>
       <c r="G12" s="27" t="s">
-        <v>14</v>
+        <v>239</v>
       </c>
       <c r="H12" s="27"/>
       <c r="I12" s="27"/>
-      <c r="J12" s="30"/>
-    </row>
-    <row r="13" spans="1:16" ht="120">
-      <c r="A13" s="26">
-        <v>10</v>
+      <c r="J12" s="32"/>
+    </row>
+    <row r="13" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="28">
+        <v>11</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>209</v>
+        <v>245</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>210</v>
+        <v>246</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>211</v>
+        <v>247</v>
       </c>
       <c r="E13" s="27" t="s">
-        <v>208</v>
+        <v>237</v>
       </c>
       <c r="F13" s="27" t="s">
-        <v>101</v>
+        <v>238</v>
       </c>
       <c r="G13" s="27" t="s">
-        <v>14</v>
+        <v>239</v>
       </c>
       <c r="H13" s="27"/>
       <c r="I13" s="27"/>
-      <c r="J13" s="30"/>
-    </row>
-    <row r="14" spans="1:16" ht="120">
+      <c r="J13" s="32"/>
+    </row>
+    <row r="14" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="26">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14" s="27" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>213</v>
-      </c>
-      <c r="D14" s="27" t="s">
-        <v>214</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="D14" s="27"/>
       <c r="E14" s="27" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="F14" s="27" t="s">
-        <v>101</v>
+        <v>203</v>
       </c>
       <c r="G14" s="27" t="s">
         <v>14</v>
@@ -3165,47 +3239,35 @@
       <c r="I14" s="27"/>
       <c r="J14" s="30"/>
     </row>
-    <row r="15" spans="1:16" ht="90">
-      <c r="A15" s="26">
-        <v>12</v>
-      </c>
-      <c r="B15" s="27" t="s">
-        <v>215</v>
-      </c>
-      <c r="C15" s="27" t="s">
-        <v>216</v>
-      </c>
-      <c r="D15" s="27" t="s">
-        <v>217</v>
-      </c>
-      <c r="E15" s="27" t="s">
-        <v>218</v>
-      </c>
-      <c r="F15" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="G15" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="H15" s="27"/>
-      <c r="I15" s="27"/>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
       <c r="J15" s="30"/>
     </row>
-    <row r="16" spans="1:16" ht="90">
+    <row r="16" spans="1:16" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" s="26">
         <v>13</v>
       </c>
       <c r="B16" s="27" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="C16" s="27" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="D16" s="27" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="E16" s="27" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="F16" s="27" t="s">
         <v>101</v>
@@ -3217,24 +3279,24 @@
       <c r="I16" s="27"/>
       <c r="J16" s="30"/>
     </row>
-    <row r="17" spans="1:10" ht="90">
+    <row r="17" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="26">
         <v>14</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="C17" s="27" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="D17" s="27" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="E17" s="27" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="F17" s="27" t="s">
-        <v>194</v>
+        <v>101</v>
       </c>
       <c r="G17" s="27" t="s">
         <v>14</v>
@@ -3243,24 +3305,24 @@
       <c r="I17" s="27"/>
       <c r="J17" s="30"/>
     </row>
-    <row r="18" spans="1:10" ht="60">
+    <row r="18" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="26">
         <v>15</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="C18" s="27" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="D18" s="27" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="E18" s="27" t="s">
-        <v>228</v>
+        <v>207</v>
       </c>
       <c r="F18" s="27" t="s">
-        <v>229</v>
+        <v>101</v>
       </c>
       <c r="G18" s="27" t="s">
         <v>14</v>
@@ -3269,38 +3331,50 @@
       <c r="I18" s="27"/>
       <c r="J18" s="30"/>
     </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="35" t="s">
-        <v>230</v>
-      </c>
-      <c r="B19" s="35"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="35"/>
-      <c r="J19" s="36"/>
-    </row>
-    <row r="20" spans="1:10" ht="90">
+    <row r="19" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A19" s="26">
+        <v>16</v>
+      </c>
+      <c r="B19" s="27" t="s">
+        <v>214</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>215</v>
+      </c>
+      <c r="D19" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="E19" s="27" t="s">
+        <v>217</v>
+      </c>
+      <c r="F19" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="G19" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="30"/>
+    </row>
+    <row r="20" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="26">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="D20" s="27" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="E20" s="27" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
       <c r="F20" s="27" t="s">
-        <v>234</v>
+        <v>101</v>
       </c>
       <c r="G20" s="27" t="s">
         <v>14</v>
@@ -3309,65 +3383,101 @@
       <c r="I20" s="27"/>
       <c r="J20" s="30"/>
     </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="30">
-        <v>17</v>
-      </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
+    <row r="21" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A21" s="26">
+        <v>18</v>
+      </c>
+      <c r="B21" s="27" t="s">
+        <v>221</v>
+      </c>
+      <c r="C21" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="D21" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="E21" s="27" t="s">
+        <v>217</v>
+      </c>
+      <c r="F21" s="27" t="s">
+        <v>193</v>
+      </c>
+      <c r="G21" s="27" t="s">
+        <v>14</v>
+      </c>
       <c r="H21" s="27"/>
       <c r="I21" s="27"/>
       <c r="J21" s="30"/>
     </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="30">
-        <v>18</v>
-      </c>
-      <c r="B22" s="27"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
+    <row r="22" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="26">
+        <v>19</v>
+      </c>
+      <c r="B22" s="27" t="s">
+        <v>224</v>
+      </c>
+      <c r="C22" s="27" t="s">
+        <v>225</v>
+      </c>
+      <c r="D22" s="27" t="s">
+        <v>226</v>
+      </c>
+      <c r="E22" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="F22" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="G22" s="27" t="s">
+        <v>14</v>
+      </c>
       <c r="H22" s="27"/>
       <c r="I22" s="27"/>
       <c r="J22" s="30"/>
     </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="30">
-        <v>19</v>
-      </c>
-      <c r="B23" s="27"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27"/>
-      <c r="I23" s="27"/>
-      <c r="J23" s="30"/>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="30">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="36" t="s">
+        <v>229</v>
+      </c>
+      <c r="B23" s="36"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="36"/>
+      <c r="J23" s="37"/>
+    </row>
+    <row r="24" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A24" s="26">
         <v>20</v>
       </c>
-      <c r="B24" s="27"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
+      <c r="B24" s="27" t="s">
+        <v>230</v>
+      </c>
+      <c r="C24" s="27" t="s">
+        <v>231</v>
+      </c>
+      <c r="D24" s="27" t="s">
+        <v>226</v>
+      </c>
+      <c r="E24" s="27" t="s">
+        <v>232</v>
+      </c>
+      <c r="F24" s="27" t="s">
+        <v>233</v>
+      </c>
+      <c r="G24" s="27" t="s">
+        <v>14</v>
+      </c>
       <c r="H24" s="27"/>
       <c r="I24" s="27"/>
       <c r="J24" s="30"/>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="30">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B25" s="27"/>
       <c r="C25" s="27"/>
@@ -3379,10 +3489,66 @@
       <c r="I25" s="27"/>
       <c r="J25" s="30"/>
     </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="30">
+        <v>18</v>
+      </c>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="27"/>
+      <c r="J26" s="30"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="30">
+        <v>19</v>
+      </c>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="27"/>
+      <c r="J27" s="30"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="30">
+        <v>20</v>
+      </c>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="27"/>
+      <c r="J28" s="30"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="30">
+        <v>21</v>
+      </c>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="30"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A11:I11"/>
-    <mergeCell ref="A19:J19"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="A23:J23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3397,9 +3563,9 @@
       <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="60">
+    <row r="1" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3438,6 +3604,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C39443884A93AC4288025566ACBEDC04" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="09db1439c13fea15c4b073f8145b668d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="dcc1e875-6396-4c7a-abb6-a5f631e4ec10" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e59e1d6e6415753d6d52256061396b9c" ns3:_="">
     <xsd:import namespace="dcc1e875-6396-4c7a-abb6-a5f631e4ec10"/>
@@ -3583,29 +3764,37 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBA5D94B-3A63-40A0-B06E-DB465E339872}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D953D7D-21BA-4E19-B5C7-89EF6D73758B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A44003BB-794C-4304-B3AC-C854D3CC3F88}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A44003BB-794C-4304-B3AC-C854D3CC3F88}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D953D7D-21BA-4E19-B5C7-89EF6D73758B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBA5D94B-3A63-40A0-B06E-DB465E339872}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="dcc1e875-6396-4c7a-abb6-a5f631e4ec10"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated Test Cases for Courses
</commit_message>
<xml_diff>
--- a/Test Cases/Test Cases.xlsx
+++ b/Test Cases/Test Cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University stuff\AssignmentOrganizer\Test Cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Projects\CS372-AssignmentOrganizer\Test Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1639DA9-9DB3-4D41-B554-43E4432EB8D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1753BEBB-82D3-4D2B-A073-21ED67226BC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HomePage" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -1562,17 +1561,17 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="25" style="1" customWidth="1"/>
-    <col min="3" max="4" width="24.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="38.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="41.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="3" max="4" width="24.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="38.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="41.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1601,7 +1600,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -1630,7 +1629,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="30">
         <v>2</v>
       </c>
@@ -1659,7 +1658,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="30">
         <v>3</v>
       </c>
@@ -1688,7 +1687,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="30">
         <v>4</v>
       </c>
@@ -1713,7 +1712,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="30">
         <v>5</v>
       </c>
@@ -1742,7 +1741,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="30">
         <v>6</v>
       </c>
@@ -1771,7 +1770,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="30">
         <v>7</v>
       </c>
@@ -1800,7 +1799,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="30">
         <v>8</v>
       </c>
@@ -1829,7 +1828,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="30">
         <v>9</v>
       </c>
@@ -1858,7 +1857,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <v>10</v>
       </c>
@@ -1887,7 +1886,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13"/>
       <c r="B12" s="9"/>
       <c r="C12" s="13" t="s">
@@ -1912,7 +1911,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13"/>
       <c r="B13" s="9"/>
       <c r="C13" s="13" t="s">
@@ -1937,7 +1936,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="13"/>
       <c r="B14" s="9"/>
       <c r="C14" s="13" t="s">
@@ -1962,7 +1961,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="15"/>
       <c r="B15" s="16"/>
       <c r="C15" s="15" t="s">
@@ -2001,19 +2000,19 @@
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
-    <col min="5" max="5" width="31.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" customWidth="1"/>
+    <col min="5" max="5" width="31.44140625" customWidth="1"/>
     <col min="6" max="6" width="25" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" customWidth="1"/>
-    <col min="9" max="9" width="7.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" customWidth="1"/>
+    <col min="9" max="9" width="7.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2042,7 +2041,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
         <v>63</v>
       </c>
@@ -2055,7 +2054,7 @@
       <c r="H2" s="33"/>
       <c r="I2" s="33"/>
     </row>
-    <row r="3" spans="1:9" s="21" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="21" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="18">
         <v>1</v>
       </c>
@@ -2082,7 +2081,7 @@
       </c>
       <c r="I3" s="19"/>
     </row>
-    <row r="4" spans="1:9" s="21" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" s="21" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="18">
         <v>2</v>
       </c>
@@ -2109,7 +2108,7 @@
       </c>
       <c r="I4" s="19"/>
     </row>
-    <row r="5" spans="1:9" s="21" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="21" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="18">
         <v>3</v>
       </c>
@@ -2136,7 +2135,7 @@
       </c>
       <c r="I5" s="19"/>
     </row>
-    <row r="6" spans="1:9" s="21" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" s="21" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="18">
         <v>4</v>
       </c>
@@ -2163,7 +2162,7 @@
       </c>
       <c r="I6" s="19"/>
     </row>
-    <row r="7" spans="1:9" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="21" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="18">
         <v>5</v>
       </c>
@@ -2190,7 +2189,7 @@
       </c>
       <c r="I7" s="19"/>
     </row>
-    <row r="8" spans="1:9" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" s="21" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="18">
         <v>6</v>
       </c>
@@ -2217,7 +2216,7 @@
       </c>
       <c r="I8" s="19"/>
     </row>
-    <row r="9" spans="1:9" s="21" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" s="21" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="28">
         <v>7</v>
       </c>
@@ -2244,7 +2243,7 @@
       </c>
       <c r="I9" s="19"/>
     </row>
-    <row r="10" spans="1:9" s="21" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" s="21" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="31">
         <v>8</v>
       </c>
@@ -2269,7 +2268,7 @@
       <c r="H10" s="19"/>
       <c r="I10" s="19"/>
     </row>
-    <row r="11" spans="1:9" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" s="21" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="28">
         <v>9</v>
       </c>
@@ -2294,7 +2293,7 @@
       <c r="H11" s="19"/>
       <c r="I11" s="19"/>
     </row>
-    <row r="12" spans="1:9" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="34" t="s">
         <v>107</v>
       </c>
@@ -2307,7 +2306,7 @@
       <c r="H12" s="34"/>
       <c r="I12" s="34"/>
     </row>
-    <row r="13" spans="1:9" s="21" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" s="21" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A13" s="18">
         <v>10</v>
       </c>
@@ -2334,7 +2333,7 @@
       </c>
       <c r="I13" s="19"/>
     </row>
-    <row r="14" spans="1:9" s="21" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" s="21" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A14" s="18">
         <v>11</v>
       </c>
@@ -2361,7 +2360,7 @@
       </c>
       <c r="I14" s="19"/>
     </row>
-    <row r="15" spans="1:9" s="21" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" s="21" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A15" s="18">
         <v>12</v>
       </c>
@@ -2388,7 +2387,7 @@
       </c>
       <c r="I15" s="19"/>
     </row>
-    <row r="16" spans="1:9" s="21" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" s="21" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A16" s="18">
         <v>13</v>
       </c>
@@ -2415,7 +2414,7 @@
       </c>
       <c r="I16" s="19"/>
     </row>
-    <row r="17" spans="1:9" s="21" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" s="21" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A17" s="28">
         <v>14</v>
       </c>
@@ -2442,7 +2441,7 @@
       </c>
       <c r="I17" s="19"/>
     </row>
-    <row r="18" spans="1:9" s="21" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" s="21" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A18" s="18">
         <v>15</v>
       </c>
@@ -2469,7 +2468,7 @@
       </c>
       <c r="I18" s="19"/>
     </row>
-    <row r="19" spans="1:9" s="21" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" s="21" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="18">
         <v>16</v>
       </c>
@@ -2496,7 +2495,7 @@
       </c>
       <c r="I19" s="19"/>
     </row>
-    <row r="20" spans="1:9" s="21" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" s="21" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="18">
         <v>17</v>
       </c>
@@ -2523,7 +2522,7 @@
       </c>
       <c r="I20" s="19"/>
     </row>
-    <row r="21" spans="1:9" s="21" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" s="21" customFormat="1" ht="19.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="34" t="s">
         <v>146</v>
       </c>
@@ -2538,7 +2537,7 @@
       </c>
       <c r="I21" s="34"/>
     </row>
-    <row r="22" spans="1:9" s="21" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" s="21" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A22" s="18">
         <v>18</v>
       </c>
@@ -2565,7 +2564,7 @@
       </c>
       <c r="I22" s="19"/>
     </row>
-    <row r="23" spans="1:9" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" s="21" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="18">
         <v>19</v>
       </c>
@@ -2590,7 +2589,7 @@
       </c>
       <c r="I23" s="19"/>
     </row>
-    <row r="24" spans="1:9" s="21" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" s="21" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A24" s="18">
         <v>20</v>
       </c>
@@ -2617,7 +2616,7 @@
       </c>
       <c r="I24" s="19"/>
     </row>
-    <row r="25" spans="1:9" s="21" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" s="21" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A25" s="18">
         <v>21</v>
       </c>
@@ -2644,7 +2643,7 @@
       </c>
       <c r="I25" s="19"/>
     </row>
-    <row r="26" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="23"/>
       <c r="B26" s="22"/>
       <c r="C26" s="22"/>
@@ -2655,7 +2654,7 @@
       <c r="H26" s="22"/>
       <c r="I26" s="22"/>
     </row>
-    <row r="27" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="23"/>
       <c r="B27" s="22"/>
       <c r="C27" s="22"/>
@@ -2666,7 +2665,7 @@
       <c r="H27" s="22"/>
       <c r="I27" s="22"/>
     </row>
-    <row r="28" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="23"/>
       <c r="B28" s="22"/>
       <c r="C28" s="22"/>
@@ -2677,7 +2676,7 @@
       <c r="H28" s="22"/>
       <c r="I28" s="22"/>
     </row>
-    <row r="29" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="23"/>
       <c r="B29" s="22"/>
       <c r="C29" s="22"/>
@@ -2688,7 +2687,7 @@
       <c r="H29" s="22"/>
       <c r="I29" s="22"/>
     </row>
-    <row r="30" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="23"/>
       <c r="B30" s="22"/>
       <c r="C30" s="22"/>
@@ -2699,7 +2698,7 @@
       <c r="H30" s="22"/>
       <c r="I30" s="22"/>
     </row>
-    <row r="31" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="23"/>
       <c r="B31" s="22"/>
       <c r="C31" s="22"/>
@@ -2710,7 +2709,7 @@
       <c r="H31" s="22"/>
       <c r="I31" s="22"/>
     </row>
-    <row r="32" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="23"/>
       <c r="B32" s="22"/>
       <c r="C32" s="22"/>
@@ -2721,7 +2720,7 @@
       <c r="H32" s="22"/>
       <c r="I32" s="22"/>
     </row>
-    <row r="33" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="9"/>
       <c r="B33" s="22"/>
       <c r="C33" s="22"/>
@@ -2732,7 +2731,7 @@
       <c r="H33" s="22"/>
       <c r="I33" s="22"/>
     </row>
-    <row r="34" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="9"/>
       <c r="B34" s="22"/>
       <c r="C34" s="22"/>
@@ -2743,7 +2742,7 @@
       <c r="H34" s="22"/>
       <c r="I34" s="22"/>
     </row>
-    <row r="35" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="9"/>
       <c r="B35" s="22"/>
       <c r="C35" s="22"/>
@@ -2754,7 +2753,7 @@
       <c r="H35" s="22"/>
       <c r="I35" s="22"/>
     </row>
-    <row r="36" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="9"/>
       <c r="B36" s="22"/>
       <c r="C36" s="22"/>
@@ -2765,7 +2764,7 @@
       <c r="H36" s="22"/>
       <c r="I36" s="22"/>
     </row>
-    <row r="37" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="9"/>
       <c r="B37" s="22"/>
       <c r="C37" s="22"/>
@@ -2776,7 +2775,7 @@
       <c r="H37" s="22"/>
       <c r="I37" s="22"/>
     </row>
-    <row r="38" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="9"/>
       <c r="B38" s="22"/>
       <c r="C38" s="22"/>
@@ -2787,7 +2786,7 @@
       <c r="H38" s="22"/>
       <c r="I38" s="22"/>
     </row>
-    <row r="39" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="9"/>
       <c r="B39" s="22"/>
       <c r="C39" s="22"/>
@@ -2798,7 +2797,7 @@
       <c r="H39" s="22"/>
       <c r="I39" s="22"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="24"/>
       <c r="B40" s="25"/>
       <c r="C40" s="25"/>
@@ -2809,7 +2808,7 @@
       <c r="H40" s="25"/>
       <c r="I40" s="25"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="24"/>
       <c r="B41" s="25"/>
       <c r="C41" s="25"/>
@@ -2820,7 +2819,7 @@
       <c r="H41" s="25"/>
       <c r="I41" s="25"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="24"/>
       <c r="B42" s="25"/>
       <c r="C42" s="25"/>
@@ -2846,25 +2845,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
-    <col min="4" max="4" width="31.28515625" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" customWidth="1"/>
+    <col min="4" max="4" width="31.33203125" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" customWidth="1"/>
-    <col min="10" max="10" width="17.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" customWidth="1"/>
+    <col min="10" max="10" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2896,7 +2895,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="26">
         <v>1</v>
       </c>
@@ -2927,7 +2926,7 @@
       <c r="O2" s="21"/>
       <c r="P2" s="21"/>
     </row>
-    <row r="3" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="26">
         <v>2</v>
       </c>
@@ -2953,7 +2952,7 @@
       <c r="I3" s="27"/>
       <c r="J3" s="30"/>
     </row>
-    <row r="4" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="26">
         <v>3</v>
       </c>
@@ -2979,8 +2978,10 @@
       <c r="I4" s="27"/>
       <c r="J4" s="30"/>
     </row>
-    <row r="5" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
+    <row r="5" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="26">
+        <v>4</v>
+      </c>
       <c r="B5" s="27" t="s">
         <v>234</v>
       </c>
@@ -3003,9 +3004,9 @@
       <c r="I5" s="27"/>
       <c r="J5" s="30"/>
     </row>
-    <row r="6" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="26">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="27" t="s">
         <v>180</v>
@@ -3029,9 +3030,9 @@
       <c r="I6" s="27"/>
       <c r="J6" s="30"/>
     </row>
-    <row r="7" spans="1:16" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="28">
-        <v>5</v>
+    <row r="7" spans="1:16" ht="72" x14ac:dyDescent="0.3">
+      <c r="A7" s="26">
+        <v>6</v>
       </c>
       <c r="B7" s="27" t="s">
         <v>184</v>
@@ -3057,9 +3058,9 @@
         <v>188</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="26">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="27" t="s">
         <v>189</v>
@@ -3083,9 +3084,9 @@
       <c r="I8" s="27"/>
       <c r="J8" s="30"/>
     </row>
-    <row r="9" spans="1:16" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="28">
-        <v>7</v>
+    <row r="9" spans="1:16" ht="72" x14ac:dyDescent="0.3">
+      <c r="A9" s="26">
+        <v>8</v>
       </c>
       <c r="B9" s="27" t="s">
         <v>194</v>
@@ -3111,9 +3112,9 @@
         <v>199</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="75" x14ac:dyDescent="0.25">
-      <c r="A10" s="28">
-        <v>8</v>
+    <row r="10" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="26">
+        <v>9</v>
       </c>
       <c r="B10" s="27" t="s">
         <v>248</v>
@@ -3137,9 +3138,9 @@
       <c r="I10" s="27"/>
       <c r="J10" s="32"/>
     </row>
-    <row r="11" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="28">
-        <v>9</v>
+    <row r="11" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="26">
+        <v>10</v>
       </c>
       <c r="B11" s="27" t="s">
         <v>240</v>
@@ -3163,9 +3164,9 @@
       <c r="I11" s="27"/>
       <c r="J11" s="32"/>
     </row>
-    <row r="12" spans="1:16" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="28">
-        <v>10</v>
+    <row r="12" spans="1:16" ht="72" x14ac:dyDescent="0.3">
+      <c r="A12" s="26">
+        <v>11</v>
       </c>
       <c r="B12" s="27" t="s">
         <v>235</v>
@@ -3189,9 +3190,9 @@
       <c r="I12" s="27"/>
       <c r="J12" s="32"/>
     </row>
-    <row r="13" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="28">
-        <v>11</v>
+    <row r="13" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="26">
+        <v>12</v>
       </c>
       <c r="B13" s="27" t="s">
         <v>245</v>
@@ -3215,9 +3216,9 @@
       <c r="I13" s="27"/>
       <c r="J13" s="32"/>
     </row>
-    <row r="14" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="26">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="27" t="s">
         <v>200</v>
@@ -3239,7 +3240,7 @@
       <c r="I14" s="27"/>
       <c r="J14" s="30"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="35" t="s">
         <v>107</v>
       </c>
@@ -3253,9 +3254,9 @@
       <c r="I15" s="35"/>
       <c r="J15" s="30"/>
     </row>
-    <row r="16" spans="1:16" ht="90" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A16" s="26">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B16" s="27" t="s">
         <v>204</v>
@@ -3279,9 +3280,9 @@
       <c r="I16" s="27"/>
       <c r="J16" s="30"/>
     </row>
-    <row r="17" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A17" s="26">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B17" s="27" t="s">
         <v>208</v>
@@ -3305,9 +3306,9 @@
       <c r="I17" s="27"/>
       <c r="J17" s="30"/>
     </row>
-    <row r="18" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A18" s="26">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B18" s="27" t="s">
         <v>211</v>
@@ -3331,9 +3332,9 @@
       <c r="I18" s="27"/>
       <c r="J18" s="30"/>
     </row>
-    <row r="19" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A19" s="26">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B19" s="27" t="s">
         <v>214</v>
@@ -3357,9 +3358,9 @@
       <c r="I19" s="27"/>
       <c r="J19" s="30"/>
     </row>
-    <row r="20" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A20" s="26">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B20" s="27" t="s">
         <v>218</v>
@@ -3383,9 +3384,9 @@
       <c r="I20" s="27"/>
       <c r="J20" s="30"/>
     </row>
-    <row r="21" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A21" s="26">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B21" s="27" t="s">
         <v>221</v>
@@ -3409,9 +3410,9 @@
       <c r="I21" s="27"/>
       <c r="J21" s="30"/>
     </row>
-    <row r="22" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="26">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B22" s="27" t="s">
         <v>224</v>
@@ -3435,7 +3436,7 @@
       <c r="I22" s="27"/>
       <c r="J22" s="30"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="36" t="s">
         <v>229</v>
       </c>
@@ -3449,9 +3450,9 @@
       <c r="I23" s="36"/>
       <c r="J23" s="37"/>
     </row>
-    <row r="24" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A24" s="26">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B24" s="27" t="s">
         <v>230</v>
@@ -3475,9 +3476,9 @@
       <c r="I24" s="27"/>
       <c r="J24" s="30"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="30">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B25" s="27"/>
       <c r="C25" s="27"/>
@@ -3489,9 +3490,9 @@
       <c r="I25" s="27"/>
       <c r="J25" s="30"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="30">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B26" s="27"/>
       <c r="C26" s="27"/>
@@ -3503,9 +3504,9 @@
       <c r="I26" s="27"/>
       <c r="J26" s="30"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="30">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B27" s="27"/>
       <c r="C27" s="27"/>
@@ -3517,9 +3518,9 @@
       <c r="I27" s="27"/>
       <c r="J27" s="30"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="30">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B28" s="27"/>
       <c r="C28" s="27"/>
@@ -3531,9 +3532,9 @@
       <c r="I28" s="27"/>
       <c r="J28" s="30"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="30">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B29" s="27"/>
       <c r="C29" s="27"/>
@@ -3563,9 +3564,9 @@
       <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3604,21 +3605,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C39443884A93AC4288025566ACBEDC04" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="09db1439c13fea15c4b073f8145b668d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="dcc1e875-6396-4c7a-abb6-a5f631e4ec10" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e59e1d6e6415753d6d52256061396b9c" ns3:_="">
     <xsd:import namespace="dcc1e875-6396-4c7a-abb6-a5f631e4ec10"/>
@@ -3764,24 +3750,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D953D7D-21BA-4E19-B5C7-89EF6D73758B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A44003BB-794C-4304-B3AC-C854D3CC3F88}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBA5D94B-3A63-40A0-B06E-DB465E339872}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3797,4 +3781,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A44003BB-794C-4304-B3AC-C854D3CC3F88}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D953D7D-21BA-4E19-B5C7-89EF6D73758B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Test cases conflict resolution
</commit_message>
<xml_diff>
--- a/Test Cases/Test Cases.xlsx
+++ b/Test Cases/Test Cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Projects\CS372-AssignmentOrganizer\Test Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F9D08333-1EE8-43B9-A5C4-098A5947D53A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1753BEBB-82D3-4D2B-A073-21ED67226BC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HomePage" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,16 @@
     <sheet name="CoursesPage" sheetId="3" r:id="rId3"/>
     <sheet name="AssignmentsPage" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029" iterateDelta="1E-4"/>
+  <calcPr calcId="191028" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -28,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="253">
   <si>
     <t>Test Case#</t>
   </si>
@@ -568,9 +576,6 @@
   </si>
   <si>
     <t>Results should show up as soon as letter is typed in.</t>
-  </si>
-  <si>
-    <t>Select semster from the drop down.</t>
   </si>
   <si>
     <t>Enter a semester in the database.</t>
@@ -759,6 +764,68 @@
   </si>
   <si>
     <t xml:space="preserve">It gets deleted. A pop up confirms the deletion to the user and it's deleted in the Json file. </t>
+  </si>
+  <si>
+    <t>Select semester from the drop down.</t>
+  </si>
+  <si>
+    <t>Adding an existing course code with different character cases.</t>
+  </si>
+  <si>
+    <t>1.Choose a semester.
+2.Enter a course code different letter cases
+3.Existing course name same letter cases</t>
+  </si>
+  <si>
+    <t>A dialogue shouls appear telling user course code already exist.</t>
+  </si>
+  <si>
+    <t>Adds the course to the semester</t>
+  </si>
+  <si>
+    <t>Dose not work</t>
+  </si>
+  <si>
+    <t>Adding an existing course to a semester with matching cases</t>
+  </si>
+  <si>
+    <t>Semester: Fall 2019, Course Code: cs-200, Course Name: Intro to DBMS.</t>
+  </si>
+  <si>
+    <t>Semester: Fall 2019, Course Code: CS-200, Course Name: Intro to DBMS.</t>
+  </si>
+  <si>
+    <t>A dialogue shouls appear telling user course already exist.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A warning dialogue box appeared. </t>
+  </si>
+  <si>
+    <t>Adding an existing course name with different character cases.</t>
+  </si>
+  <si>
+    <t>1.Choose a semester.
+2.Existing course code
+3.Existing course name differnt letter cases</t>
+  </si>
+  <si>
+    <t>Semester: Fall 2019, Course Code: CS-200, Course Name: intro to dbms.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adding a valid course spelling existing semester name in lower case or a different case sequence </t>
+  </si>
+  <si>
+    <t>1. Type semester term and year                   2.Enter a course code
+3.Enter a course name</t>
+  </si>
+  <si>
+    <t>1. fall 2019:MATH-100: Intro to Calculus                                                    2.fALL 2019:ENGL-100:Critical Read and Writing1</t>
+  </si>
+  <si>
+    <t>Result to appear in existing course list</t>
+  </si>
+  <si>
+    <t>A warning dialogue popped up saying semesters dose not exist</t>
   </si>
 </sst>
 </file>
@@ -991,7 +1058,7 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1084,6 +1151,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1491,17 +1561,17 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="25" style="1" customWidth="1"/>
-    <col min="3" max="4" width="24.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="38.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="41.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="3" max="4" width="24.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="38.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="41.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1530,7 +1600,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -1559,7 +1629,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="30">
         <v>2</v>
       </c>
@@ -1588,7 +1658,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="30">
         <v>3</v>
       </c>
@@ -1617,7 +1687,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="30">
         <v>4</v>
       </c>
@@ -1642,7 +1712,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="30">
         <v>5</v>
       </c>
@@ -1671,7 +1741,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="30">
         <v>6</v>
       </c>
@@ -1700,7 +1770,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="30">
         <v>7</v>
       </c>
@@ -1729,7 +1799,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="30">
         <v>8</v>
       </c>
@@ -1758,7 +1828,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="30">
         <v>9</v>
       </c>
@@ -1787,7 +1857,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <v>10</v>
       </c>
@@ -1816,7 +1886,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13"/>
       <c r="B12" s="9"/>
       <c r="C12" s="13" t="s">
@@ -1841,7 +1911,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13"/>
       <c r="B13" s="9"/>
       <c r="C13" s="13" t="s">
@@ -1866,7 +1936,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="13"/>
       <c r="B14" s="9"/>
       <c r="C14" s="13" t="s">
@@ -1891,7 +1961,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="15"/>
       <c r="B15" s="16"/>
       <c r="C15" s="15" t="s">
@@ -1930,19 +2000,19 @@
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
-    <col min="5" max="5" width="31.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" customWidth="1"/>
+    <col min="5" max="5" width="31.44140625" customWidth="1"/>
     <col min="6" max="6" width="25" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" customWidth="1"/>
-    <col min="9" max="9" width="7.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" customWidth="1"/>
+    <col min="9" max="9" width="7.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1971,20 +2041,20 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+    <row r="2" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-    </row>
-    <row r="3" spans="1:9" s="21" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+    </row>
+    <row r="3" spans="1:9" s="21" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="18">
         <v>1</v>
       </c>
@@ -2011,7 +2081,7 @@
       </c>
       <c r="I3" s="19"/>
     </row>
-    <row r="4" spans="1:9" s="21" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" s="21" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="18">
         <v>2</v>
       </c>
@@ -2038,7 +2108,7 @@
       </c>
       <c r="I4" s="19"/>
     </row>
-    <row r="5" spans="1:9" s="21" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="21" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="18">
         <v>3</v>
       </c>
@@ -2065,7 +2135,7 @@
       </c>
       <c r="I5" s="19"/>
     </row>
-    <row r="6" spans="1:9" s="21" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" s="21" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="18">
         <v>4</v>
       </c>
@@ -2092,7 +2162,7 @@
       </c>
       <c r="I6" s="19"/>
     </row>
-    <row r="7" spans="1:9" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="21" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="18">
         <v>5</v>
       </c>
@@ -2119,7 +2189,7 @@
       </c>
       <c r="I7" s="19"/>
     </row>
-    <row r="8" spans="1:9" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" s="21" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="18">
         <v>6</v>
       </c>
@@ -2146,7 +2216,7 @@
       </c>
       <c r="I8" s="19"/>
     </row>
-    <row r="9" spans="1:9" s="21" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" s="21" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="28">
         <v>7</v>
       </c>
@@ -2173,7 +2243,7 @@
       </c>
       <c r="I9" s="19"/>
     </row>
-    <row r="10" spans="1:9" s="21" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" s="21" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="31">
         <v>8</v>
       </c>
@@ -2198,7 +2268,7 @@
       <c r="H10" s="19"/>
       <c r="I10" s="19"/>
     </row>
-    <row r="11" spans="1:9" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" s="21" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="28">
         <v>9</v>
       </c>
@@ -2223,20 +2293,20 @@
       <c r="H11" s="19"/>
       <c r="I11" s="19"/>
     </row>
-    <row r="12" spans="1:9" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="33" t="s">
+    <row r="12" spans="1:9" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="B12" s="33"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-    </row>
-    <row r="13" spans="1:9" s="21" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+    </row>
+    <row r="13" spans="1:9" s="21" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A13" s="18">
         <v>10</v>
       </c>
@@ -2263,7 +2333,7 @@
       </c>
       <c r="I13" s="19"/>
     </row>
-    <row r="14" spans="1:9" s="21" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" s="21" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A14" s="18">
         <v>11</v>
       </c>
@@ -2290,7 +2360,7 @@
       </c>
       <c r="I14" s="19"/>
     </row>
-    <row r="15" spans="1:9" s="21" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" s="21" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A15" s="18">
         <v>12</v>
       </c>
@@ -2317,7 +2387,7 @@
       </c>
       <c r="I15" s="19"/>
     </row>
-    <row r="16" spans="1:9" s="21" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" s="21" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A16" s="18">
         <v>13</v>
       </c>
@@ -2344,7 +2414,7 @@
       </c>
       <c r="I16" s="19"/>
     </row>
-    <row r="17" spans="1:9" s="21" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" s="21" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A17" s="28">
         <v>14</v>
       </c>
@@ -2371,7 +2441,7 @@
       </c>
       <c r="I17" s="19"/>
     </row>
-    <row r="18" spans="1:9" s="21" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" s="21" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A18" s="18">
         <v>15</v>
       </c>
@@ -2398,7 +2468,7 @@
       </c>
       <c r="I18" s="19"/>
     </row>
-    <row r="19" spans="1:9" s="21" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" s="21" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="18">
         <v>16</v>
       </c>
@@ -2425,7 +2495,7 @@
       </c>
       <c r="I19" s="19"/>
     </row>
-    <row r="20" spans="1:9" s="21" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" s="21" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="18">
         <v>17</v>
       </c>
@@ -2452,22 +2522,22 @@
       </c>
       <c r="I20" s="19"/>
     </row>
-    <row r="21" spans="1:9" s="21" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="33" t="s">
+    <row r="21" spans="1:9" s="21" customFormat="1" ht="19.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="B21" s="33"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="I21" s="33"/>
-    </row>
-    <row r="22" spans="1:9" s="21" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" s="34"/>
+    </row>
+    <row r="22" spans="1:9" s="21" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A22" s="18">
         <v>18</v>
       </c>
@@ -2494,7 +2564,7 @@
       </c>
       <c r="I22" s="19"/>
     </row>
-    <row r="23" spans="1:9" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" s="21" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="18">
         <v>19</v>
       </c>
@@ -2519,7 +2589,7 @@
       </c>
       <c r="I23" s="19"/>
     </row>
-    <row r="24" spans="1:9" s="21" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" s="21" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A24" s="18">
         <v>20</v>
       </c>
@@ -2546,7 +2616,7 @@
       </c>
       <c r="I24" s="19"/>
     </row>
-    <row r="25" spans="1:9" s="21" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" s="21" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A25" s="18">
         <v>21</v>
       </c>
@@ -2573,7 +2643,7 @@
       </c>
       <c r="I25" s="19"/>
     </row>
-    <row r="26" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="23"/>
       <c r="B26" s="22"/>
       <c r="C26" s="22"/>
@@ -2584,7 +2654,7 @@
       <c r="H26" s="22"/>
       <c r="I26" s="22"/>
     </row>
-    <row r="27" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="23"/>
       <c r="B27" s="22"/>
       <c r="C27" s="22"/>
@@ -2595,7 +2665,7 @@
       <c r="H27" s="22"/>
       <c r="I27" s="22"/>
     </row>
-    <row r="28" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="23"/>
       <c r="B28" s="22"/>
       <c r="C28" s="22"/>
@@ -2606,7 +2676,7 @@
       <c r="H28" s="22"/>
       <c r="I28" s="22"/>
     </row>
-    <row r="29" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="23"/>
       <c r="B29" s="22"/>
       <c r="C29" s="22"/>
@@ -2617,7 +2687,7 @@
       <c r="H29" s="22"/>
       <c r="I29" s="22"/>
     </row>
-    <row r="30" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="23"/>
       <c r="B30" s="22"/>
       <c r="C30" s="22"/>
@@ -2628,7 +2698,7 @@
       <c r="H30" s="22"/>
       <c r="I30" s="22"/>
     </row>
-    <row r="31" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="23"/>
       <c r="B31" s="22"/>
       <c r="C31" s="22"/>
@@ -2639,7 +2709,7 @@
       <c r="H31" s="22"/>
       <c r="I31" s="22"/>
     </row>
-    <row r="32" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="23"/>
       <c r="B32" s="22"/>
       <c r="C32" s="22"/>
@@ -2650,7 +2720,7 @@
       <c r="H32" s="22"/>
       <c r="I32" s="22"/>
     </row>
-    <row r="33" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="9"/>
       <c r="B33" s="22"/>
       <c r="C33" s="22"/>
@@ -2661,7 +2731,7 @@
       <c r="H33" s="22"/>
       <c r="I33" s="22"/>
     </row>
-    <row r="34" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="9"/>
       <c r="B34" s="22"/>
       <c r="C34" s="22"/>
@@ -2672,7 +2742,7 @@
       <c r="H34" s="22"/>
       <c r="I34" s="22"/>
     </row>
-    <row r="35" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="9"/>
       <c r="B35" s="22"/>
       <c r="C35" s="22"/>
@@ -2683,7 +2753,7 @@
       <c r="H35" s="22"/>
       <c r="I35" s="22"/>
     </row>
-    <row r="36" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="9"/>
       <c r="B36" s="22"/>
       <c r="C36" s="22"/>
@@ -2694,7 +2764,7 @@
       <c r="H36" s="22"/>
       <c r="I36" s="22"/>
     </row>
-    <row r="37" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="9"/>
       <c r="B37" s="22"/>
       <c r="C37" s="22"/>
@@ -2705,7 +2775,7 @@
       <c r="H37" s="22"/>
       <c r="I37" s="22"/>
     </row>
-    <row r="38" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="9"/>
       <c r="B38" s="22"/>
       <c r="C38" s="22"/>
@@ -2716,7 +2786,7 @@
       <c r="H38" s="22"/>
       <c r="I38" s="22"/>
     </row>
-    <row r="39" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="9"/>
       <c r="B39" s="22"/>
       <c r="C39" s="22"/>
@@ -2727,7 +2797,7 @@
       <c r="H39" s="22"/>
       <c r="I39" s="22"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="24"/>
       <c r="B40" s="25"/>
       <c r="C40" s="25"/>
@@ -2738,7 +2808,7 @@
       <c r="H40" s="25"/>
       <c r="I40" s="25"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="24"/>
       <c r="B41" s="25"/>
       <c r="C41" s="25"/>
@@ -2749,7 +2819,7 @@
       <c r="H41" s="25"/>
       <c r="I41" s="25"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="24"/>
       <c r="B42" s="25"/>
       <c r="C42" s="25"/>
@@ -2773,27 +2843,27 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:P25"/>
+  <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
-    <col min="4" max="4" width="31.28515625" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" customWidth="1"/>
+    <col min="4" max="4" width="31.33203125" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" customWidth="1"/>
-    <col min="10" max="10" width="17.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" customWidth="1"/>
+    <col min="10" max="10" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2825,7 +2895,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="26">
         <v>1</v>
       </c>
@@ -2856,7 +2926,7 @@
       <c r="O2" s="21"/>
       <c r="P2" s="21"/>
     </row>
-    <row r="3" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="26">
         <v>2</v>
       </c>
@@ -2882,7 +2952,7 @@
       <c r="I3" s="27"/>
       <c r="J3" s="30"/>
     </row>
-    <row r="4" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="26">
         <v>3</v>
       </c>
@@ -2908,21 +2978,21 @@
       <c r="I4" s="27"/>
       <c r="J4" s="30"/>
     </row>
-    <row r="5" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="26">
         <v>4</v>
       </c>
       <c r="B5" s="27" t="s">
+        <v>234</v>
+      </c>
+      <c r="C5" s="27" t="s">
         <v>177</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="D5" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="E5" s="27" t="s">
         <v>179</v>
-      </c>
-      <c r="E5" s="27" t="s">
-        <v>180</v>
       </c>
       <c r="F5" s="27" t="s">
         <v>101</v>
@@ -2934,21 +3004,21 @@
       <c r="I5" s="27"/>
       <c r="J5" s="30"/>
     </row>
-    <row r="6" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="26">
         <v>5</v>
       </c>
       <c r="B6" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="C6" s="27" t="s">
         <v>181</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="D6" s="27" t="s">
         <v>182</v>
       </c>
-      <c r="D6" s="27" t="s">
+      <c r="E6" s="27" t="s">
         <v>183</v>
-      </c>
-      <c r="E6" s="27" t="s">
-        <v>184</v>
       </c>
       <c r="F6" s="27" t="s">
         <v>101</v>
@@ -2960,24 +3030,24 @@
       <c r="I6" s="27"/>
       <c r="J6" s="30"/>
     </row>
-    <row r="7" spans="1:16" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="28">
+    <row r="7" spans="1:16" ht="72" x14ac:dyDescent="0.3">
+      <c r="A7" s="26">
         <v>6</v>
       </c>
       <c r="B7" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>181</v>
+      </c>
+      <c r="D7" s="27" t="s">
         <v>185</v>
       </c>
-      <c r="C7" s="27" t="s">
-        <v>182</v>
-      </c>
-      <c r="D7" s="27" t="s">
+      <c r="E7" s="27" t="s">
         <v>186</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="F7" s="27" t="s">
         <v>187</v>
-      </c>
-      <c r="F7" s="27" t="s">
-        <v>188</v>
       </c>
       <c r="G7" s="27" t="s">
         <v>96</v>
@@ -2985,27 +3055,27 @@
       <c r="H7" s="27"/>
       <c r="I7" s="27"/>
       <c r="J7" s="30" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="75" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="26">
         <v>7</v>
       </c>
       <c r="B8" s="27" t="s">
+        <v>189</v>
+      </c>
+      <c r="C8" s="27" t="s">
         <v>190</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="D8" s="27" t="s">
         <v>191</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="E8" s="27" t="s">
         <v>192</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="F8" s="27" t="s">
         <v>193</v>
-      </c>
-      <c r="F8" s="27" t="s">
-        <v>194</v>
       </c>
       <c r="G8" s="27" t="s">
         <v>14</v>
@@ -3014,24 +3084,24 @@
       <c r="I8" s="27"/>
       <c r="J8" s="30"/>
     </row>
-    <row r="9" spans="1:16" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="28">
+    <row r="9" spans="1:16" ht="72" x14ac:dyDescent="0.3">
+      <c r="A9" s="26">
         <v>8</v>
       </c>
       <c r="B9" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="C9" s="27" t="s">
         <v>195</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="D9" s="27" t="s">
         <v>196</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="E9" s="27" t="s">
         <v>197</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="F9" s="27" t="s">
         <v>198</v>
-      </c>
-      <c r="F9" s="27" t="s">
-        <v>199</v>
       </c>
       <c r="G9" s="27" t="s">
         <v>96</v>
@@ -3039,117 +3109,129 @@
       <c r="H9" s="27"/>
       <c r="I9" s="27"/>
       <c r="J9" s="30" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="26">
         <v>9</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>201</v>
+        <v>248</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>202</v>
-      </c>
-      <c r="D10" s="27"/>
+        <v>249</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>250</v>
+      </c>
       <c r="E10" s="27" t="s">
-        <v>203</v>
+        <v>251</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>204</v>
+        <v>252</v>
       </c>
       <c r="G10" s="27" t="s">
-        <v>14</v>
+        <v>239</v>
       </c>
       <c r="H10" s="27"/>
       <c r="I10" s="27"/>
-      <c r="J10" s="30"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
-        <v>107</v>
-      </c>
-      <c r="B11" s="34"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="30"/>
-    </row>
-    <row r="12" spans="1:16" ht="90" x14ac:dyDescent="0.25">
+      <c r="J10" s="32"/>
+    </row>
+    <row r="11" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="26">
+        <v>10</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>240</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>181</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>242</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>243</v>
+      </c>
+      <c r="F11" s="27" t="s">
+        <v>244</v>
+      </c>
+      <c r="G11" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="32"/>
+    </row>
+    <row r="12" spans="1:16" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" s="26">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>205</v>
+        <v>235</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>206</v>
+        <v>236</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>207</v>
+        <v>241</v>
       </c>
       <c r="E12" s="27" t="s">
-        <v>208</v>
+        <v>237</v>
       </c>
       <c r="F12" s="27" t="s">
-        <v>101</v>
+        <v>238</v>
       </c>
       <c r="G12" s="27" t="s">
-        <v>14</v>
+        <v>239</v>
       </c>
       <c r="H12" s="27"/>
       <c r="I12" s="27"/>
-      <c r="J12" s="30"/>
-    </row>
-    <row r="13" spans="1:16" ht="90" x14ac:dyDescent="0.25">
+      <c r="J12" s="32"/>
+    </row>
+    <row r="13" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="26">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>209</v>
+        <v>245</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>210</v>
+        <v>246</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>211</v>
+        <v>247</v>
       </c>
       <c r="E13" s="27" t="s">
-        <v>208</v>
+        <v>237</v>
       </c>
       <c r="F13" s="27" t="s">
-        <v>101</v>
+        <v>238</v>
       </c>
       <c r="G13" s="27" t="s">
-        <v>14</v>
+        <v>239</v>
       </c>
       <c r="H13" s="27"/>
       <c r="I13" s="27"/>
-      <c r="J13" s="30"/>
-    </row>
-    <row r="14" spans="1:16" ht="90" x14ac:dyDescent="0.25">
+      <c r="J13" s="32"/>
+    </row>
+    <row r="14" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="26">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="27" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>213</v>
-      </c>
-      <c r="D14" s="27" t="s">
-        <v>214</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="D14" s="27"/>
       <c r="E14" s="27" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="F14" s="27" t="s">
-        <v>101</v>
+        <v>203</v>
       </c>
       <c r="G14" s="27" t="s">
         <v>14</v>
@@ -3158,47 +3240,35 @@
       <c r="I14" s="27"/>
       <c r="J14" s="30"/>
     </row>
-    <row r="15" spans="1:16" ht="90" x14ac:dyDescent="0.25">
-      <c r="A15" s="26">
-        <v>13</v>
-      </c>
-      <c r="B15" s="27" t="s">
-        <v>215</v>
-      </c>
-      <c r="C15" s="27" t="s">
-        <v>216</v>
-      </c>
-      <c r="D15" s="27" t="s">
-        <v>217</v>
-      </c>
-      <c r="E15" s="27" t="s">
-        <v>218</v>
-      </c>
-      <c r="F15" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="G15" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="H15" s="27"/>
-      <c r="I15" s="27"/>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
       <c r="J15" s="30"/>
     </row>
-    <row r="16" spans="1:16" ht="90" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A16" s="26">
         <v>14</v>
       </c>
       <c r="B16" s="27" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="C16" s="27" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="D16" s="27" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="E16" s="27" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="F16" s="27" t="s">
         <v>101</v>
@@ -3210,24 +3280,24 @@
       <c r="I16" s="27"/>
       <c r="J16" s="30"/>
     </row>
-    <row r="17" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A17" s="26">
         <v>15</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="C17" s="27" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="D17" s="27" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="E17" s="27" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="F17" s="27" t="s">
-        <v>194</v>
+        <v>101</v>
       </c>
       <c r="G17" s="27" t="s">
         <v>14</v>
@@ -3236,24 +3306,24 @@
       <c r="I17" s="27"/>
       <c r="J17" s="30"/>
     </row>
-    <row r="18" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A18" s="26">
         <v>16</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="C18" s="27" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="D18" s="27" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="E18" s="27" t="s">
-        <v>228</v>
+        <v>207</v>
       </c>
       <c r="F18" s="27" t="s">
-        <v>229</v>
+        <v>101</v>
       </c>
       <c r="G18" s="27" t="s">
         <v>14</v>
@@ -3262,38 +3332,50 @@
       <c r="I18" s="27"/>
       <c r="J18" s="30"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="35" t="s">
-        <v>230</v>
-      </c>
-      <c r="B19" s="35"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="35"/>
-      <c r="J19" s="36"/>
-    </row>
-    <row r="20" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A19" s="26">
+        <v>17</v>
+      </c>
+      <c r="B19" s="27" t="s">
+        <v>214</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>215</v>
+      </c>
+      <c r="D19" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="E19" s="27" t="s">
+        <v>217</v>
+      </c>
+      <c r="F19" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="G19" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="30"/>
+    </row>
+    <row r="20" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A20" s="26">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="D20" s="27" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="E20" s="27" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
       <c r="F20" s="27" t="s">
-        <v>234</v>
+        <v>101</v>
       </c>
       <c r="G20" s="27" t="s">
         <v>14</v>
@@ -3302,65 +3384,101 @@
       <c r="I20" s="27"/>
       <c r="J20" s="30"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="30">
-        <v>17</v>
-      </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
+    <row r="21" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A21" s="26">
+        <v>19</v>
+      </c>
+      <c r="B21" s="27" t="s">
+        <v>221</v>
+      </c>
+      <c r="C21" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="D21" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="E21" s="27" t="s">
+        <v>217</v>
+      </c>
+      <c r="F21" s="27" t="s">
+        <v>193</v>
+      </c>
+      <c r="G21" s="27" t="s">
+        <v>14</v>
+      </c>
       <c r="H21" s="27"/>
       <c r="I21" s="27"/>
       <c r="J21" s="30"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="30">
-        <v>18</v>
-      </c>
-      <c r="B22" s="27"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
+    <row r="22" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="26">
+        <v>20</v>
+      </c>
+      <c r="B22" s="27" t="s">
+        <v>224</v>
+      </c>
+      <c r="C22" s="27" t="s">
+        <v>225</v>
+      </c>
+      <c r="D22" s="27" t="s">
+        <v>226</v>
+      </c>
+      <c r="E22" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="F22" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="G22" s="27" t="s">
+        <v>14</v>
+      </c>
       <c r="H22" s="27"/>
       <c r="I22" s="27"/>
       <c r="J22" s="30"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="30">
-        <v>19</v>
-      </c>
-      <c r="B23" s="27"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27"/>
-      <c r="I23" s="27"/>
-      <c r="J23" s="30"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="30">
-        <v>20</v>
-      </c>
-      <c r="B24" s="27"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="36" t="s">
+        <v>229</v>
+      </c>
+      <c r="B23" s="36"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="36"/>
+      <c r="J23" s="37"/>
+    </row>
+    <row r="24" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A24" s="26">
+        <v>21</v>
+      </c>
+      <c r="B24" s="27" t="s">
+        <v>230</v>
+      </c>
+      <c r="C24" s="27" t="s">
+        <v>231</v>
+      </c>
+      <c r="D24" s="27" t="s">
+        <v>226</v>
+      </c>
+      <c r="E24" s="27" t="s">
+        <v>232</v>
+      </c>
+      <c r="F24" s="27" t="s">
+        <v>233</v>
+      </c>
+      <c r="G24" s="27" t="s">
+        <v>14</v>
+      </c>
       <c r="H24" s="27"/>
       <c r="I24" s="27"/>
       <c r="J24" s="30"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="30">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B25" s="27"/>
       <c r="C25" s="27"/>
@@ -3372,10 +3490,66 @@
       <c r="I25" s="27"/>
       <c r="J25" s="30"/>
     </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="30">
+        <v>23</v>
+      </c>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="27"/>
+      <c r="J26" s="30"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="30">
+        <v>24</v>
+      </c>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="27"/>
+      <c r="J27" s="30"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="30">
+        <v>25</v>
+      </c>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="27"/>
+      <c r="J28" s="30"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="30">
+        <v>26</v>
+      </c>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="30"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A11:I11"/>
-    <mergeCell ref="A19:J19"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="A23:J23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3390,9 +3564,9 @@
       <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3612,15 +3786,8 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A44003BB-794C-4304-B3AC-C854D3CC3F88}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="dcc1e875-6396-4c7a-abb6-a5f631e4ec10"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Test cases conflict resolution (#61)
</commit_message>
<xml_diff>
--- a/Test Cases/Test Cases.xlsx
+++ b/Test Cases/Test Cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Projects\CS372-AssignmentOrganizer\Test Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F9D08333-1EE8-43B9-A5C4-098A5947D53A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1753BEBB-82D3-4D2B-A073-21ED67226BC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HomePage" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,16 @@
     <sheet name="CoursesPage" sheetId="3" r:id="rId3"/>
     <sheet name="AssignmentsPage" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029" iterateDelta="1E-4"/>
+  <calcPr calcId="191028" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -28,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="253">
   <si>
     <t>Test Case#</t>
   </si>
@@ -568,9 +576,6 @@
   </si>
   <si>
     <t>Results should show up as soon as letter is typed in.</t>
-  </si>
-  <si>
-    <t>Select semster from the drop down.</t>
   </si>
   <si>
     <t>Enter a semester in the database.</t>
@@ -759,6 +764,68 @@
   </si>
   <si>
     <t xml:space="preserve">It gets deleted. A pop up confirms the deletion to the user and it's deleted in the Json file. </t>
+  </si>
+  <si>
+    <t>Select semester from the drop down.</t>
+  </si>
+  <si>
+    <t>Adding an existing course code with different character cases.</t>
+  </si>
+  <si>
+    <t>1.Choose a semester.
+2.Enter a course code different letter cases
+3.Existing course name same letter cases</t>
+  </si>
+  <si>
+    <t>A dialogue shouls appear telling user course code already exist.</t>
+  </si>
+  <si>
+    <t>Adds the course to the semester</t>
+  </si>
+  <si>
+    <t>Dose not work</t>
+  </si>
+  <si>
+    <t>Adding an existing course to a semester with matching cases</t>
+  </si>
+  <si>
+    <t>Semester: Fall 2019, Course Code: cs-200, Course Name: Intro to DBMS.</t>
+  </si>
+  <si>
+    <t>Semester: Fall 2019, Course Code: CS-200, Course Name: Intro to DBMS.</t>
+  </si>
+  <si>
+    <t>A dialogue shouls appear telling user course already exist.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A warning dialogue box appeared. </t>
+  </si>
+  <si>
+    <t>Adding an existing course name with different character cases.</t>
+  </si>
+  <si>
+    <t>1.Choose a semester.
+2.Existing course code
+3.Existing course name differnt letter cases</t>
+  </si>
+  <si>
+    <t>Semester: Fall 2019, Course Code: CS-200, Course Name: intro to dbms.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adding a valid course spelling existing semester name in lower case or a different case sequence </t>
+  </si>
+  <si>
+    <t>1. Type semester term and year                   2.Enter a course code
+3.Enter a course name</t>
+  </si>
+  <si>
+    <t>1. fall 2019:MATH-100: Intro to Calculus                                                    2.fALL 2019:ENGL-100:Critical Read and Writing1</t>
+  </si>
+  <si>
+    <t>Result to appear in existing course list</t>
+  </si>
+  <si>
+    <t>A warning dialogue popped up saying semesters dose not exist</t>
   </si>
 </sst>
 </file>
@@ -991,7 +1058,7 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1084,6 +1151,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1491,17 +1561,17 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="25" style="1" customWidth="1"/>
-    <col min="3" max="4" width="24.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="38.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="41.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="3" max="4" width="24.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="38.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="41.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1530,7 +1600,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -1559,7 +1629,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="30">
         <v>2</v>
       </c>
@@ -1588,7 +1658,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="30">
         <v>3</v>
       </c>
@@ -1617,7 +1687,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="30">
         <v>4</v>
       </c>
@@ -1642,7 +1712,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="30">
         <v>5</v>
       </c>
@@ -1671,7 +1741,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="30">
         <v>6</v>
       </c>
@@ -1700,7 +1770,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="30">
         <v>7</v>
       </c>
@@ -1729,7 +1799,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="30">
         <v>8</v>
       </c>
@@ -1758,7 +1828,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="30">
         <v>9</v>
       </c>
@@ -1787,7 +1857,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <v>10</v>
       </c>
@@ -1816,7 +1886,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13"/>
       <c r="B12" s="9"/>
       <c r="C12" s="13" t="s">
@@ -1841,7 +1911,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13"/>
       <c r="B13" s="9"/>
       <c r="C13" s="13" t="s">
@@ -1866,7 +1936,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="13"/>
       <c r="B14" s="9"/>
       <c r="C14" s="13" t="s">
@@ -1891,7 +1961,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="15"/>
       <c r="B15" s="16"/>
       <c r="C15" s="15" t="s">
@@ -1930,19 +2000,19 @@
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
-    <col min="5" max="5" width="31.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" customWidth="1"/>
+    <col min="5" max="5" width="31.44140625" customWidth="1"/>
     <col min="6" max="6" width="25" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" customWidth="1"/>
-    <col min="9" max="9" width="7.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" customWidth="1"/>
+    <col min="9" max="9" width="7.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1971,20 +2041,20 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+    <row r="2" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-    </row>
-    <row r="3" spans="1:9" s="21" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+    </row>
+    <row r="3" spans="1:9" s="21" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="18">
         <v>1</v>
       </c>
@@ -2011,7 +2081,7 @@
       </c>
       <c r="I3" s="19"/>
     </row>
-    <row r="4" spans="1:9" s="21" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" s="21" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="18">
         <v>2</v>
       </c>
@@ -2038,7 +2108,7 @@
       </c>
       <c r="I4" s="19"/>
     </row>
-    <row r="5" spans="1:9" s="21" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="21" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="18">
         <v>3</v>
       </c>
@@ -2065,7 +2135,7 @@
       </c>
       <c r="I5" s="19"/>
     </row>
-    <row r="6" spans="1:9" s="21" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" s="21" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="18">
         <v>4</v>
       </c>
@@ -2092,7 +2162,7 @@
       </c>
       <c r="I6" s="19"/>
     </row>
-    <row r="7" spans="1:9" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="21" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="18">
         <v>5</v>
       </c>
@@ -2119,7 +2189,7 @@
       </c>
       <c r="I7" s="19"/>
     </row>
-    <row r="8" spans="1:9" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" s="21" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="18">
         <v>6</v>
       </c>
@@ -2146,7 +2216,7 @@
       </c>
       <c r="I8" s="19"/>
     </row>
-    <row r="9" spans="1:9" s="21" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" s="21" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="28">
         <v>7</v>
       </c>
@@ -2173,7 +2243,7 @@
       </c>
       <c r="I9" s="19"/>
     </row>
-    <row r="10" spans="1:9" s="21" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" s="21" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="31">
         <v>8</v>
       </c>
@@ -2198,7 +2268,7 @@
       <c r="H10" s="19"/>
       <c r="I10" s="19"/>
     </row>
-    <row r="11" spans="1:9" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" s="21" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="28">
         <v>9</v>
       </c>
@@ -2223,20 +2293,20 @@
       <c r="H11" s="19"/>
       <c r="I11" s="19"/>
     </row>
-    <row r="12" spans="1:9" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="33" t="s">
+    <row r="12" spans="1:9" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="B12" s="33"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-    </row>
-    <row r="13" spans="1:9" s="21" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+    </row>
+    <row r="13" spans="1:9" s="21" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A13" s="18">
         <v>10</v>
       </c>
@@ -2263,7 +2333,7 @@
       </c>
       <c r="I13" s="19"/>
     </row>
-    <row r="14" spans="1:9" s="21" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" s="21" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A14" s="18">
         <v>11</v>
       </c>
@@ -2290,7 +2360,7 @@
       </c>
       <c r="I14" s="19"/>
     </row>
-    <row r="15" spans="1:9" s="21" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" s="21" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A15" s="18">
         <v>12</v>
       </c>
@@ -2317,7 +2387,7 @@
       </c>
       <c r="I15" s="19"/>
     </row>
-    <row r="16" spans="1:9" s="21" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" s="21" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A16" s="18">
         <v>13</v>
       </c>
@@ -2344,7 +2414,7 @@
       </c>
       <c r="I16" s="19"/>
     </row>
-    <row r="17" spans="1:9" s="21" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" s="21" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A17" s="28">
         <v>14</v>
       </c>
@@ -2371,7 +2441,7 @@
       </c>
       <c r="I17" s="19"/>
     </row>
-    <row r="18" spans="1:9" s="21" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" s="21" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A18" s="18">
         <v>15</v>
       </c>
@@ -2398,7 +2468,7 @@
       </c>
       <c r="I18" s="19"/>
     </row>
-    <row r="19" spans="1:9" s="21" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" s="21" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="18">
         <v>16</v>
       </c>
@@ -2425,7 +2495,7 @@
       </c>
       <c r="I19" s="19"/>
     </row>
-    <row r="20" spans="1:9" s="21" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" s="21" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="18">
         <v>17</v>
       </c>
@@ -2452,22 +2522,22 @@
       </c>
       <c r="I20" s="19"/>
     </row>
-    <row r="21" spans="1:9" s="21" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="33" t="s">
+    <row r="21" spans="1:9" s="21" customFormat="1" ht="19.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="B21" s="33"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="I21" s="33"/>
-    </row>
-    <row r="22" spans="1:9" s="21" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" s="34"/>
+    </row>
+    <row r="22" spans="1:9" s="21" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A22" s="18">
         <v>18</v>
       </c>
@@ -2494,7 +2564,7 @@
       </c>
       <c r="I22" s="19"/>
     </row>
-    <row r="23" spans="1:9" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" s="21" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="18">
         <v>19</v>
       </c>
@@ -2519,7 +2589,7 @@
       </c>
       <c r="I23" s="19"/>
     </row>
-    <row r="24" spans="1:9" s="21" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" s="21" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A24" s="18">
         <v>20</v>
       </c>
@@ -2546,7 +2616,7 @@
       </c>
       <c r="I24" s="19"/>
     </row>
-    <row r="25" spans="1:9" s="21" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" s="21" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A25" s="18">
         <v>21</v>
       </c>
@@ -2573,7 +2643,7 @@
       </c>
       <c r="I25" s="19"/>
     </row>
-    <row r="26" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="23"/>
       <c r="B26" s="22"/>
       <c r="C26" s="22"/>
@@ -2584,7 +2654,7 @@
       <c r="H26" s="22"/>
       <c r="I26" s="22"/>
     </row>
-    <row r="27" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="23"/>
       <c r="B27" s="22"/>
       <c r="C27" s="22"/>
@@ -2595,7 +2665,7 @@
       <c r="H27" s="22"/>
       <c r="I27" s="22"/>
     </row>
-    <row r="28" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="23"/>
       <c r="B28" s="22"/>
       <c r="C28" s="22"/>
@@ -2606,7 +2676,7 @@
       <c r="H28" s="22"/>
       <c r="I28" s="22"/>
     </row>
-    <row r="29" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="23"/>
       <c r="B29" s="22"/>
       <c r="C29" s="22"/>
@@ -2617,7 +2687,7 @@
       <c r="H29" s="22"/>
       <c r="I29" s="22"/>
     </row>
-    <row r="30" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="23"/>
       <c r="B30" s="22"/>
       <c r="C30" s="22"/>
@@ -2628,7 +2698,7 @@
       <c r="H30" s="22"/>
       <c r="I30" s="22"/>
     </row>
-    <row r="31" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="23"/>
       <c r="B31" s="22"/>
       <c r="C31" s="22"/>
@@ -2639,7 +2709,7 @@
       <c r="H31" s="22"/>
       <c r="I31" s="22"/>
     </row>
-    <row r="32" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="23"/>
       <c r="B32" s="22"/>
       <c r="C32" s="22"/>
@@ -2650,7 +2720,7 @@
       <c r="H32" s="22"/>
       <c r="I32" s="22"/>
     </row>
-    <row r="33" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="9"/>
       <c r="B33" s="22"/>
       <c r="C33" s="22"/>
@@ -2661,7 +2731,7 @@
       <c r="H33" s="22"/>
       <c r="I33" s="22"/>
     </row>
-    <row r="34" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="9"/>
       <c r="B34" s="22"/>
       <c r="C34" s="22"/>
@@ -2672,7 +2742,7 @@
       <c r="H34" s="22"/>
       <c r="I34" s="22"/>
     </row>
-    <row r="35" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="9"/>
       <c r="B35" s="22"/>
       <c r="C35" s="22"/>
@@ -2683,7 +2753,7 @@
       <c r="H35" s="22"/>
       <c r="I35" s="22"/>
     </row>
-    <row r="36" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="9"/>
       <c r="B36" s="22"/>
       <c r="C36" s="22"/>
@@ -2694,7 +2764,7 @@
       <c r="H36" s="22"/>
       <c r="I36" s="22"/>
     </row>
-    <row r="37" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="9"/>
       <c r="B37" s="22"/>
       <c r="C37" s="22"/>
@@ -2705,7 +2775,7 @@
       <c r="H37" s="22"/>
       <c r="I37" s="22"/>
     </row>
-    <row r="38" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="9"/>
       <c r="B38" s="22"/>
       <c r="C38" s="22"/>
@@ -2716,7 +2786,7 @@
       <c r="H38" s="22"/>
       <c r="I38" s="22"/>
     </row>
-    <row r="39" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="9"/>
       <c r="B39" s="22"/>
       <c r="C39" s="22"/>
@@ -2727,7 +2797,7 @@
       <c r="H39" s="22"/>
       <c r="I39" s="22"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="24"/>
       <c r="B40" s="25"/>
       <c r="C40" s="25"/>
@@ -2738,7 +2808,7 @@
       <c r="H40" s="25"/>
       <c r="I40" s="25"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="24"/>
       <c r="B41" s="25"/>
       <c r="C41" s="25"/>
@@ -2749,7 +2819,7 @@
       <c r="H41" s="25"/>
       <c r="I41" s="25"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="24"/>
       <c r="B42" s="25"/>
       <c r="C42" s="25"/>
@@ -2773,27 +2843,27 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:P25"/>
+  <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
-    <col min="4" max="4" width="31.28515625" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" customWidth="1"/>
+    <col min="4" max="4" width="31.33203125" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" customWidth="1"/>
-    <col min="10" max="10" width="17.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" customWidth="1"/>
+    <col min="10" max="10" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2825,7 +2895,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="26">
         <v>1</v>
       </c>
@@ -2856,7 +2926,7 @@
       <c r="O2" s="21"/>
       <c r="P2" s="21"/>
     </row>
-    <row r="3" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="26">
         <v>2</v>
       </c>
@@ -2882,7 +2952,7 @@
       <c r="I3" s="27"/>
       <c r="J3" s="30"/>
     </row>
-    <row r="4" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="26">
         <v>3</v>
       </c>
@@ -2908,21 +2978,21 @@
       <c r="I4" s="27"/>
       <c r="J4" s="30"/>
     </row>
-    <row r="5" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="26">
         <v>4</v>
       </c>
       <c r="B5" s="27" t="s">
+        <v>234</v>
+      </c>
+      <c r="C5" s="27" t="s">
         <v>177</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="D5" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="E5" s="27" t="s">
         <v>179</v>
-      </c>
-      <c r="E5" s="27" t="s">
-        <v>180</v>
       </c>
       <c r="F5" s="27" t="s">
         <v>101</v>
@@ -2934,21 +3004,21 @@
       <c r="I5" s="27"/>
       <c r="J5" s="30"/>
     </row>
-    <row r="6" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="26">
         <v>5</v>
       </c>
       <c r="B6" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="C6" s="27" t="s">
         <v>181</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="D6" s="27" t="s">
         <v>182</v>
       </c>
-      <c r="D6" s="27" t="s">
+      <c r="E6" s="27" t="s">
         <v>183</v>
-      </c>
-      <c r="E6" s="27" t="s">
-        <v>184</v>
       </c>
       <c r="F6" s="27" t="s">
         <v>101</v>
@@ -2960,24 +3030,24 @@
       <c r="I6" s="27"/>
       <c r="J6" s="30"/>
     </row>
-    <row r="7" spans="1:16" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="28">
+    <row r="7" spans="1:16" ht="72" x14ac:dyDescent="0.3">
+      <c r="A7" s="26">
         <v>6</v>
       </c>
       <c r="B7" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>181</v>
+      </c>
+      <c r="D7" s="27" t="s">
         <v>185</v>
       </c>
-      <c r="C7" s="27" t="s">
-        <v>182</v>
-      </c>
-      <c r="D7" s="27" t="s">
+      <c r="E7" s="27" t="s">
         <v>186</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="F7" s="27" t="s">
         <v>187</v>
-      </c>
-      <c r="F7" s="27" t="s">
-        <v>188</v>
       </c>
       <c r="G7" s="27" t="s">
         <v>96</v>
@@ -2985,27 +3055,27 @@
       <c r="H7" s="27"/>
       <c r="I7" s="27"/>
       <c r="J7" s="30" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="75" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="26">
         <v>7</v>
       </c>
       <c r="B8" s="27" t="s">
+        <v>189</v>
+      </c>
+      <c r="C8" s="27" t="s">
         <v>190</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="D8" s="27" t="s">
         <v>191</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="E8" s="27" t="s">
         <v>192</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="F8" s="27" t="s">
         <v>193</v>
-      </c>
-      <c r="F8" s="27" t="s">
-        <v>194</v>
       </c>
       <c r="G8" s="27" t="s">
         <v>14</v>
@@ -3014,24 +3084,24 @@
       <c r="I8" s="27"/>
       <c r="J8" s="30"/>
     </row>
-    <row r="9" spans="1:16" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="28">
+    <row r="9" spans="1:16" ht="72" x14ac:dyDescent="0.3">
+      <c r="A9" s="26">
         <v>8</v>
       </c>
       <c r="B9" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="C9" s="27" t="s">
         <v>195</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="D9" s="27" t="s">
         <v>196</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="E9" s="27" t="s">
         <v>197</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="F9" s="27" t="s">
         <v>198</v>
-      </c>
-      <c r="F9" s="27" t="s">
-        <v>199</v>
       </c>
       <c r="G9" s="27" t="s">
         <v>96</v>
@@ -3039,117 +3109,129 @@
       <c r="H9" s="27"/>
       <c r="I9" s="27"/>
       <c r="J9" s="30" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="26">
         <v>9</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>201</v>
+        <v>248</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>202</v>
-      </c>
-      <c r="D10" s="27"/>
+        <v>249</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>250</v>
+      </c>
       <c r="E10" s="27" t="s">
-        <v>203</v>
+        <v>251</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>204</v>
+        <v>252</v>
       </c>
       <c r="G10" s="27" t="s">
-        <v>14</v>
+        <v>239</v>
       </c>
       <c r="H10" s="27"/>
       <c r="I10" s="27"/>
-      <c r="J10" s="30"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
-        <v>107</v>
-      </c>
-      <c r="B11" s="34"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="30"/>
-    </row>
-    <row r="12" spans="1:16" ht="90" x14ac:dyDescent="0.25">
+      <c r="J10" s="32"/>
+    </row>
+    <row r="11" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="26">
+        <v>10</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>240</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>181</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>242</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>243</v>
+      </c>
+      <c r="F11" s="27" t="s">
+        <v>244</v>
+      </c>
+      <c r="G11" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="32"/>
+    </row>
+    <row r="12" spans="1:16" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" s="26">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>205</v>
+        <v>235</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>206</v>
+        <v>236</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>207</v>
+        <v>241</v>
       </c>
       <c r="E12" s="27" t="s">
-        <v>208</v>
+        <v>237</v>
       </c>
       <c r="F12" s="27" t="s">
-        <v>101</v>
+        <v>238</v>
       </c>
       <c r="G12" s="27" t="s">
-        <v>14</v>
+        <v>239</v>
       </c>
       <c r="H12" s="27"/>
       <c r="I12" s="27"/>
-      <c r="J12" s="30"/>
-    </row>
-    <row r="13" spans="1:16" ht="90" x14ac:dyDescent="0.25">
+      <c r="J12" s="32"/>
+    </row>
+    <row r="13" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="26">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>209</v>
+        <v>245</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>210</v>
+        <v>246</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>211</v>
+        <v>247</v>
       </c>
       <c r="E13" s="27" t="s">
-        <v>208</v>
+        <v>237</v>
       </c>
       <c r="F13" s="27" t="s">
-        <v>101</v>
+        <v>238</v>
       </c>
       <c r="G13" s="27" t="s">
-        <v>14</v>
+        <v>239</v>
       </c>
       <c r="H13" s="27"/>
       <c r="I13" s="27"/>
-      <c r="J13" s="30"/>
-    </row>
-    <row r="14" spans="1:16" ht="90" x14ac:dyDescent="0.25">
+      <c r="J13" s="32"/>
+    </row>
+    <row r="14" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="26">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="27" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>213</v>
-      </c>
-      <c r="D14" s="27" t="s">
-        <v>214</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="D14" s="27"/>
       <c r="E14" s="27" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="F14" s="27" t="s">
-        <v>101</v>
+        <v>203</v>
       </c>
       <c r="G14" s="27" t="s">
         <v>14</v>
@@ -3158,47 +3240,35 @@
       <c r="I14" s="27"/>
       <c r="J14" s="30"/>
     </row>
-    <row r="15" spans="1:16" ht="90" x14ac:dyDescent="0.25">
-      <c r="A15" s="26">
-        <v>13</v>
-      </c>
-      <c r="B15" s="27" t="s">
-        <v>215</v>
-      </c>
-      <c r="C15" s="27" t="s">
-        <v>216</v>
-      </c>
-      <c r="D15" s="27" t="s">
-        <v>217</v>
-      </c>
-      <c r="E15" s="27" t="s">
-        <v>218</v>
-      </c>
-      <c r="F15" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="G15" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="H15" s="27"/>
-      <c r="I15" s="27"/>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
       <c r="J15" s="30"/>
     </row>
-    <row r="16" spans="1:16" ht="90" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A16" s="26">
         <v>14</v>
       </c>
       <c r="B16" s="27" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="C16" s="27" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="D16" s="27" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="E16" s="27" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="F16" s="27" t="s">
         <v>101</v>
@@ -3210,24 +3280,24 @@
       <c r="I16" s="27"/>
       <c r="J16" s="30"/>
     </row>
-    <row r="17" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A17" s="26">
         <v>15</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="C17" s="27" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="D17" s="27" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="E17" s="27" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="F17" s="27" t="s">
-        <v>194</v>
+        <v>101</v>
       </c>
       <c r="G17" s="27" t="s">
         <v>14</v>
@@ -3236,24 +3306,24 @@
       <c r="I17" s="27"/>
       <c r="J17" s="30"/>
     </row>
-    <row r="18" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A18" s="26">
         <v>16</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="C18" s="27" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="D18" s="27" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="E18" s="27" t="s">
-        <v>228</v>
+        <v>207</v>
       </c>
       <c r="F18" s="27" t="s">
-        <v>229</v>
+        <v>101</v>
       </c>
       <c r="G18" s="27" t="s">
         <v>14</v>
@@ -3262,38 +3332,50 @@
       <c r="I18" s="27"/>
       <c r="J18" s="30"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="35" t="s">
-        <v>230</v>
-      </c>
-      <c r="B19" s="35"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="35"/>
-      <c r="J19" s="36"/>
-    </row>
-    <row r="20" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A19" s="26">
+        <v>17</v>
+      </c>
+      <c r="B19" s="27" t="s">
+        <v>214</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>215</v>
+      </c>
+      <c r="D19" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="E19" s="27" t="s">
+        <v>217</v>
+      </c>
+      <c r="F19" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="G19" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="30"/>
+    </row>
+    <row r="20" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A20" s="26">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="D20" s="27" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="E20" s="27" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
       <c r="F20" s="27" t="s">
-        <v>234</v>
+        <v>101</v>
       </c>
       <c r="G20" s="27" t="s">
         <v>14</v>
@@ -3302,65 +3384,101 @@
       <c r="I20" s="27"/>
       <c r="J20" s="30"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="30">
-        <v>17</v>
-      </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
+    <row r="21" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A21" s="26">
+        <v>19</v>
+      </c>
+      <c r="B21" s="27" t="s">
+        <v>221</v>
+      </c>
+      <c r="C21" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="D21" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="E21" s="27" t="s">
+        <v>217</v>
+      </c>
+      <c r="F21" s="27" t="s">
+        <v>193</v>
+      </c>
+      <c r="G21" s="27" t="s">
+        <v>14</v>
+      </c>
       <c r="H21" s="27"/>
       <c r="I21" s="27"/>
       <c r="J21" s="30"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="30">
-        <v>18</v>
-      </c>
-      <c r="B22" s="27"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
+    <row r="22" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="26">
+        <v>20</v>
+      </c>
+      <c r="B22" s="27" t="s">
+        <v>224</v>
+      </c>
+      <c r="C22" s="27" t="s">
+        <v>225</v>
+      </c>
+      <c r="D22" s="27" t="s">
+        <v>226</v>
+      </c>
+      <c r="E22" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="F22" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="G22" s="27" t="s">
+        <v>14</v>
+      </c>
       <c r="H22" s="27"/>
       <c r="I22" s="27"/>
       <c r="J22" s="30"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="30">
-        <v>19</v>
-      </c>
-      <c r="B23" s="27"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27"/>
-      <c r="I23" s="27"/>
-      <c r="J23" s="30"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="30">
-        <v>20</v>
-      </c>
-      <c r="B24" s="27"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="36" t="s">
+        <v>229</v>
+      </c>
+      <c r="B23" s="36"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="36"/>
+      <c r="J23" s="37"/>
+    </row>
+    <row r="24" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A24" s="26">
+        <v>21</v>
+      </c>
+      <c r="B24" s="27" t="s">
+        <v>230</v>
+      </c>
+      <c r="C24" s="27" t="s">
+        <v>231</v>
+      </c>
+      <c r="D24" s="27" t="s">
+        <v>226</v>
+      </c>
+      <c r="E24" s="27" t="s">
+        <v>232</v>
+      </c>
+      <c r="F24" s="27" t="s">
+        <v>233</v>
+      </c>
+      <c r="G24" s="27" t="s">
+        <v>14</v>
+      </c>
       <c r="H24" s="27"/>
       <c r="I24" s="27"/>
       <c r="J24" s="30"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="30">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B25" s="27"/>
       <c r="C25" s="27"/>
@@ -3372,10 +3490,66 @@
       <c r="I25" s="27"/>
       <c r="J25" s="30"/>
     </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="30">
+        <v>23</v>
+      </c>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="27"/>
+      <c r="J26" s="30"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="30">
+        <v>24</v>
+      </c>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="27"/>
+      <c r="J27" s="30"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="30">
+        <v>25</v>
+      </c>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="27"/>
+      <c r="J28" s="30"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="30">
+        <v>26</v>
+      </c>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="30"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A11:I11"/>
-    <mergeCell ref="A19:J19"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="A23:J23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3390,9 +3564,9 @@
       <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3612,15 +3786,8 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A44003BB-794C-4304-B3AC-C854D3CC3F88}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="dcc1e875-6396-4c7a-abb6-a5f631e4ec10"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>